<commit_message>
Aggiornamento ultima versione Report_CheckList
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DTSCONSULTI/DTSCONSULTINGSRL/DTSHIS/1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111DTSCONSULTI/DTSCONSULTINGSRL/DTSHIS/1.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc utente\Desktop\TestCNS\TestCNS\S1#111DTSCONSULTI\DTSHIS\1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc utente\Desktop\GATEWAY\S1#111DTSCONSULTI\DTSCONSULTINGSRL\DTSHIS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083C61AD-FE80-448B-89E0-EF06509973DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3563D163-CC11-4AE7-B4C8-50FE2DD3F3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="525">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -540,17 +540,7 @@
     <t>VALIDAZIONE_CDA2_RAD_CT22_KO</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RAD_CT23_KO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT5_KO</t>
@@ -2477,13 +2467,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T726"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomRight" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="91.7109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2535,7 +2526,7 @@
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D2" s="33"/>
       <c r="F2" s="5"/>
@@ -2560,7 +2551,7 @@
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="40" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3" s="31"/>
       <c r="F3" s="5"/>
@@ -2583,7 +2574,7 @@
       <c r="A4" s="36"/>
       <c r="B4" s="37"/>
       <c r="C4" s="40" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="4"/>
@@ -2607,7 +2598,7 @@
       <c r="A5" s="38"/>
       <c r="B5" s="39"/>
       <c r="C5" s="40" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D5" s="31"/>
       <c r="F5" s="5"/>
@@ -2745,7 +2736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>1</v>
       </c>
@@ -2765,13 +2756,13 @@
         <v>45057</v>
       </c>
       <c r="G10" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="I10" s="19" t="s">
         <v>220</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>222</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>76</v>
@@ -2789,7 +2780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>2</v>
       </c>
@@ -2809,13 +2800,13 @@
         <v>45057</v>
       </c>
       <c r="G11" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="I11" s="19" t="s">
         <v>223</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>225</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>76</v>
@@ -2833,7 +2824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>3</v>
       </c>
@@ -2853,13 +2844,13 @@
         <v>45057</v>
       </c>
       <c r="G12" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="I12" s="19" t="s">
         <v>226</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>228</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>76</v>
@@ -2877,7 +2868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>4</v>
       </c>
@@ -2897,13 +2888,13 @@
         <v>45057</v>
       </c>
       <c r="G13" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="I13" s="19" t="s">
         <v>229</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>231</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>76</v>
@@ -2921,7 +2912,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>5</v>
       </c>
@@ -2941,13 +2932,13 @@
         <v>45057</v>
       </c>
       <c r="G14" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="I14" s="19" t="s">
         <v>232</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>234</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>76</v>
@@ -2965,7 +2956,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>6</v>
       </c>
@@ -2985,13 +2976,13 @@
         <v>45063</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>76</v>
@@ -3009,7 +3000,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>7</v>
       </c>
@@ -3029,13 +3020,13 @@
         <v>45063</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>76</v>
@@ -3053,7 +3044,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
         <v>8</v>
       </c>
@@ -3073,13 +3064,13 @@
         <v>45063</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>76</v>
@@ -3097,7 +3088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>9</v>
       </c>
@@ -3117,13 +3108,13 @@
         <v>45063</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>76</v>
@@ -3141,7 +3132,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>11</v>
       </c>
@@ -3161,13 +3152,13 @@
         <v>45062</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>76</v>
@@ -3185,7 +3176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
         <v>12</v>
       </c>
@@ -3205,13 +3196,13 @@
         <v>45062</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>76</v>
@@ -3229,7 +3220,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>13</v>
       </c>
@@ -3250,10 +3241,10 @@
       <c r="H21" s="18"/>
       <c r="I21" s="23"/>
       <c r="J21" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -3267,7 +3258,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <v>14</v>
       </c>
@@ -3288,10 +3279,10 @@
       <c r="H22" s="18"/>
       <c r="I22" s="23"/>
       <c r="J22" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -3305,7 +3296,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>24</v>
       </c>
@@ -3325,13 +3316,13 @@
         <v>45063</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>76</v>
@@ -3349,7 +3340,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <v>25</v>
       </c>
@@ -3369,13 +3360,13 @@
         <v>45063</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>76</v>
@@ -3393,7 +3384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
         <v>26</v>
       </c>
@@ -3413,13 +3404,13 @@
         <v>45063</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>76</v>
@@ -3437,7 +3428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>27</v>
       </c>
@@ -3457,13 +3448,13 @@
         <v>45063</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>76</v>
@@ -3495,24 +3486,24 @@
         <v>64</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
       <c r="I27" s="19"/>
       <c r="J27" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="20"/>
@@ -3535,24 +3526,24 @@
         <v>65</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
       <c r="I28" s="23"/>
       <c r="J28" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="20"/>
@@ -3575,24 +3566,24 @@
         <v>66</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
       <c r="I29" s="23"/>
       <c r="J29" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="20"/>
@@ -3615,24 +3606,24 @@
         <v>67</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
       <c r="I30" s="19"/>
       <c r="J30" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="20"/>
@@ -3655,24 +3646,24 @@
         <v>68</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
       <c r="J31" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="20"/>
@@ -3695,19 +3686,19 @@
         <v>69</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F32" s="17">
         <v>45062</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>76</v>
@@ -3720,13 +3711,13 @@
         <v>76</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="20"/>
@@ -3749,19 +3740,19 @@
         <v>70</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F33" s="17">
         <v>45063</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>76</v>
@@ -3774,13 +3765,13 @@
         <v>76</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="20"/>
@@ -3803,22 +3794,22 @@
         <v>71</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F34" s="17">
         <v>45062</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
@@ -3828,13 +3819,13 @@
         <v>76</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O34" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="20"/>
@@ -3857,19 +3848,19 @@
         <v>72</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F35" s="17">
         <v>45062</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>76</v>
@@ -3882,13 +3873,13 @@
         <v>76</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O35" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="20"/>
@@ -3911,19 +3902,19 @@
         <v>73</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F36" s="17">
         <v>45063</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>76</v>
@@ -3936,13 +3927,13 @@
         <v>76</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O36" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="20"/>
@@ -3971,21 +3962,15 @@
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
       <c r="I37" s="19"/>
-      <c r="J37" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-      <c r="P37" s="2" t="s">
-        <v>236</v>
-      </c>
+      <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
-      <c r="R37" s="20" t="s">
-        <v>76</v>
-      </c>
+      <c r="R37" s="20"/>
       <c r="S37" s="21"/>
       <c r="T37" s="22" t="s">
         <v>24</v>
@@ -4018,7 +4003,7 @@
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="20" t="s">
@@ -4056,7 +4041,7 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Q39" s="2"/>
       <c r="R39" s="20" t="s">
@@ -4094,7 +4079,7 @@
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Q40" s="2"/>
       <c r="R40" s="20" t="s">
@@ -4132,7 +4117,7 @@
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="20" t="s">
@@ -4163,30 +4148,32 @@
         <v>45062</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
+      <c r="L42" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M42" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="20"/>
@@ -4215,30 +4202,32 @@
         <v>45062</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
+      <c r="L43" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M43" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O43" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="20"/>
@@ -4267,30 +4256,32 @@
         <v>45062</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H44" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N44" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="I44" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N44" s="2" t="s">
-        <v>248</v>
-      </c>
       <c r="O44" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q44" s="2"/>
       <c r="R44" s="20"/>
@@ -4319,30 +4310,32 @@
         <v>45062</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
+      <c r="L45" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M45" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O45" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="20"/>
@@ -4371,30 +4364,32 @@
         <v>45072</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H46" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="I46" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="I46" s="19" t="s">
-        <v>520</v>
-      </c>
       <c r="J46" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
+      <c r="L46" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M46" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q46" s="2"/>
       <c r="R46" s="20"/>
@@ -4423,30 +4418,32 @@
         <v>45062</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I47" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
+      <c r="L47" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M47" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O47" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="20"/>
@@ -4475,30 +4472,32 @@
         <v>45062</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
+      <c r="L48" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M48" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q48" s="2"/>
       <c r="R48" s="20"/>
@@ -4527,23 +4526,33 @@
         <v>45072</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
+      <c r="L49" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>270</v>
+      </c>
       <c r="Q49" s="2"/>
       <c r="R49" s="20"/>
       <c r="S49" s="21"/>
@@ -4571,30 +4580,32 @@
         <v>45062</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
+      <c r="L50" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M50" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q50" s="2"/>
       <c r="R50" s="20"/>
@@ -4623,30 +4634,32 @@
         <v>45062</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
+      <c r="L51" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M51" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O51" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q51" s="2"/>
       <c r="R51" s="20"/>
@@ -4675,23 +4688,33 @@
         <v>45072</v>
       </c>
       <c r="G52" s="18" t="s">
+        <v>522</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>523</v>
+      </c>
+      <c r="I52" s="19" t="s">
         <v>524</v>
       </c>
-      <c r="H52" s="18" t="s">
-        <v>525</v>
-      </c>
-      <c r="I52" s="19" t="s">
-        <v>526</v>
-      </c>
       <c r="J52" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
+      <c r="L52" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="O52" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>270</v>
+      </c>
       <c r="Q52" s="2"/>
       <c r="R52" s="20"/>
       <c r="S52" s="21"/>
@@ -4719,30 +4742,32 @@
         <v>45063</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
+      <c r="L53" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M53" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O53" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q53" s="2"/>
       <c r="R53" s="20"/>
@@ -4771,30 +4796,32 @@
         <v>45063</v>
       </c>
       <c r="G54" s="18" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
+      <c r="L54" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M54" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O54" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q54" s="2"/>
       <c r="R54" s="20"/>
@@ -4823,30 +4850,32 @@
         <v>45063</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
+      <c r="L55" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M55" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q55" s="2"/>
       <c r="R55" s="20"/>
@@ -4875,30 +4904,32 @@
         <v>45063</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
+      <c r="L56" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M56" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" s="20"/>
@@ -4927,30 +4958,32 @@
         <v>45063</v>
       </c>
       <c r="G57" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
+      <c r="L57" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M57" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q57" s="2"/>
       <c r="R57" s="20"/>
@@ -4979,30 +5012,32 @@
         <v>45063</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I58" s="23" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
+      <c r="L58" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M58" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O58" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" s="20"/>
@@ -5031,30 +5066,32 @@
         <v>45063</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
+      <c r="L59" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M59" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="20"/>
@@ -5083,30 +5120,32 @@
         <v>45063</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
+      <c r="L60" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M60" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O60" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="20"/>
@@ -5135,30 +5174,32 @@
         <v>45063</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
+      <c r="L61" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M61" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P61" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="20"/>
@@ -5187,30 +5228,32 @@
         <v>45063</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
+      <c r="L62" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M62" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O62" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="20"/>
@@ -5239,30 +5282,32 @@
         <v>45063</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
+      <c r="L63" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M63" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O63" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q63" s="2"/>
       <c r="R63" s="20"/>
@@ -5291,30 +5336,32 @@
         <v>45063</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
+      <c r="L64" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="M64" s="2" t="s">
         <v>76</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O64" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q64" s="2"/>
       <c r="R64" s="20"/>
@@ -5343,13 +5390,13 @@
         <v>45062</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>76</v>
@@ -5362,13 +5409,13 @@
         <v>76</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O65" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P65" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q65" s="2"/>
       <c r="R65" s="20"/>
@@ -5397,13 +5444,13 @@
         <v>45062</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>76</v>
@@ -5416,13 +5463,13 @@
         <v>76</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O66" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q66" s="2"/>
       <c r="R66" s="20"/>
@@ -5451,13 +5498,13 @@
         <v>45062</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>76</v>
@@ -5470,13 +5517,13 @@
         <v>76</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O67" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q67" s="2"/>
       <c r="R67" s="20"/>
@@ -5505,13 +5552,13 @@
         <v>45062</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I68" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>76</v>
@@ -5524,13 +5571,13 @@
         <v>76</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O68" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P68" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="20"/>
@@ -5559,13 +5606,13 @@
         <v>45062</v>
       </c>
       <c r="G69" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I69" s="23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>76</v>
@@ -5578,13 +5625,13 @@
         <v>76</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O69" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P69" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="20"/>
@@ -5613,13 +5660,13 @@
         <v>45062</v>
       </c>
       <c r="G70" s="18" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I70" s="23" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>76</v>
@@ -5632,13 +5679,13 @@
         <v>76</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O70" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="20"/>
@@ -5667,13 +5714,13 @@
         <v>45062</v>
       </c>
       <c r="G71" s="18" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I71" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>76</v>
@@ -5686,13 +5733,13 @@
         <v>76</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O71" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q71" s="2"/>
       <c r="R71" s="20"/>
@@ -5721,13 +5768,13 @@
         <v>45062</v>
       </c>
       <c r="G72" s="18" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I72" s="23" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>76</v>
@@ -5740,13 +5787,13 @@
         <v>76</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O72" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P72" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q72" s="2"/>
       <c r="R72" s="20"/>
@@ -5775,13 +5822,13 @@
         <v>45062</v>
       </c>
       <c r="G73" s="18" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I73" s="23" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>76</v>
@@ -5794,13 +5841,13 @@
         <v>76</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O73" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P73" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q73" s="2"/>
       <c r="R73" s="20"/>
@@ -5829,13 +5876,13 @@
         <v>45062</v>
       </c>
       <c r="G74" s="18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H74" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I74" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>76</v>
@@ -5848,13 +5895,13 @@
         <v>76</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O74" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P74" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q74" s="2"/>
       <c r="R74" s="20"/>
@@ -5883,13 +5930,13 @@
         <v>45062</v>
       </c>
       <c r="G75" s="18" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I75" s="23" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>76</v>
@@ -5902,13 +5949,13 @@
         <v>76</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O75" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q75" s="2"/>
       <c r="R75" s="20"/>
@@ -5937,13 +5984,13 @@
         <v>45062</v>
       </c>
       <c r="G76" s="18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H76" s="18" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I76" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>76</v>
@@ -5956,13 +6003,13 @@
         <v>76</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O76" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q76" s="2"/>
       <c r="R76" s="20"/>
@@ -5992,15 +6039,15 @@
       <c r="H77" s="18"/>
       <c r="I77" s="23"/>
       <c r="J77" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
@@ -6032,15 +6079,15 @@
       <c r="H78" s="18"/>
       <c r="I78" s="23"/>
       <c r="J78" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
@@ -6072,15 +6119,15 @@
       <c r="H79" s="18"/>
       <c r="I79" s="23"/>
       <c r="J79" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
@@ -6112,15 +6159,15 @@
       <c r="H80" s="18"/>
       <c r="I80" s="23"/>
       <c r="J80" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
       <c r="N80" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
@@ -6152,15 +6199,15 @@
       <c r="H81" s="18"/>
       <c r="I81" s="23"/>
       <c r="J81" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
@@ -6185,19 +6232,19 @@
         <v>138</v>
       </c>
       <c r="E82" s="16" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="F82" s="17">
         <v>45062</v>
       </c>
       <c r="G82" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="H82" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="I82" s="23" t="s">
         <v>313</v>
-      </c>
-      <c r="H82" s="18" t="s">
-        <v>314</v>
-      </c>
-      <c r="I82" s="23" t="s">
-        <v>315</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>76</v>
@@ -6210,13 +6257,13 @@
         <v>76</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O82" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P82" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q82" s="2"/>
       <c r="R82" s="20"/>
@@ -6236,22 +6283,22 @@
         <v>26</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E83" s="16" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="F83" s="17">
         <v>45062</v>
       </c>
       <c r="G83" s="18" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H83" s="18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I83" s="23" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>76</v>
@@ -6264,13 +6311,13 @@
         <v>76</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O83" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P83" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q83" s="2"/>
       <c r="R83" s="20"/>
@@ -6290,22 +6337,22 @@
         <v>27</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E84" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F84" s="17">
         <v>45063</v>
       </c>
       <c r="G84" s="18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H84" s="18" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I84" s="23" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>76</v>
@@ -6318,13 +6365,13 @@
         <v>76</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O84" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P84" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q84" s="2"/>
       <c r="R84" s="20"/>
@@ -6344,22 +6391,22 @@
         <v>27</v>
       </c>
       <c r="D85" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E85" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F85" s="17">
         <v>45063</v>
       </c>
       <c r="G85" s="18" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H85" s="18" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>76</v>
@@ -6372,13 +6419,13 @@
         <v>76</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O85" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P85" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q85" s="2"/>
       <c r="R85" s="20"/>
@@ -6398,22 +6445,22 @@
         <v>27</v>
       </c>
       <c r="D86" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F86" s="17">
         <v>45063</v>
       </c>
       <c r="G86" s="18" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H86" s="18" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>76</v>
@@ -6426,13 +6473,13 @@
         <v>76</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O86" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P86" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q86" s="2"/>
       <c r="R86" s="20"/>
@@ -6452,22 +6499,22 @@
         <v>27</v>
       </c>
       <c r="D87" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E87" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F87" s="17">
         <v>45063</v>
       </c>
       <c r="G87" s="18" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H87" s="18" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>76</v>
@@ -6480,13 +6527,13 @@
         <v>76</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O87" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P87" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q87" s="2"/>
       <c r="R87" s="20"/>
@@ -6506,22 +6553,22 @@
         <v>27</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E88" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F88" s="17">
         <v>45063</v>
       </c>
       <c r="G88" s="18" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H88" s="18" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I88" s="23" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>76</v>
@@ -6534,13 +6581,13 @@
         <v>76</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O88" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P88" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q88" s="2"/>
       <c r="R88" s="20"/>
@@ -6560,22 +6607,22 @@
         <v>27</v>
       </c>
       <c r="D89" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E89" s="16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F89" s="17">
         <v>45063</v>
       </c>
       <c r="G89" s="18" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H89" s="18" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I89" s="23" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>76</v>
@@ -6588,13 +6635,13 @@
         <v>76</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O89" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P89" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q89" s="2"/>
       <c r="R89" s="20"/>
@@ -6614,22 +6661,22 @@
         <v>27</v>
       </c>
       <c r="D90" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E90" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F90" s="17">
         <v>45063</v>
       </c>
       <c r="G90" s="18" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H90" s="18" t="s">
+        <v>458</v>
+      </c>
+      <c r="I90" s="23" t="s">
         <v>460</v>
-      </c>
-      <c r="I90" s="23" t="s">
-        <v>462</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>76</v>
@@ -6642,13 +6689,13 @@
         <v>76</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q90" s="2"/>
       <c r="R90" s="20"/>
@@ -6668,22 +6715,22 @@
         <v>27</v>
       </c>
       <c r="D91" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E91" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F91" s="17">
         <v>45064</v>
       </c>
       <c r="G91" s="18" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H91" s="18" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I91" s="23" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>76</v>
@@ -6696,13 +6743,13 @@
         <v>76</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O91" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P91" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q91" s="2"/>
       <c r="R91" s="20"/>
@@ -6722,22 +6769,22 @@
         <v>27</v>
       </c>
       <c r="D92" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E92" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F92" s="17">
         <v>45064</v>
       </c>
       <c r="G92" s="18" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="H92" s="18" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I92" s="23" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>76</v>
@@ -6750,13 +6797,13 @@
         <v>76</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O92" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q92" s="2"/>
       <c r="R92" s="20"/>
@@ -6776,22 +6823,22 @@
         <v>27</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E93" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F93" s="17">
         <v>45064</v>
       </c>
       <c r="G93" s="18" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H93" s="18" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I93" s="23" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>76</v>
@@ -6804,13 +6851,13 @@
         <v>76</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O93" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q93" s="2"/>
       <c r="R93" s="20"/>
@@ -6830,22 +6877,22 @@
         <v>27</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E94" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F94" s="17">
         <v>45064</v>
       </c>
       <c r="G94" s="18" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H94" s="18" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I94" s="23" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>76</v>
@@ -6858,13 +6905,13 @@
         <v>76</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O94" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P94" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q94" s="2"/>
       <c r="R94" s="20"/>
@@ -6884,22 +6931,22 @@
         <v>27</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E95" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F95" s="17">
         <v>45064</v>
       </c>
       <c r="G95" s="18" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H95" s="18" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I95" s="23" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>76</v>
@@ -6912,13 +6959,13 @@
         <v>76</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O95" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P95" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q95" s="2"/>
       <c r="R95" s="20"/>
@@ -6938,22 +6985,22 @@
         <v>27</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E96" s="16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F96" s="17">
         <v>45064</v>
       </c>
       <c r="G96" s="18" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H96" s="18" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I96" s="23" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>76</v>
@@ -6966,13 +7013,13 @@
         <v>76</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O96" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P96" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q96" s="2"/>
       <c r="R96" s="20"/>
@@ -6992,22 +7039,22 @@
         <v>27</v>
       </c>
       <c r="D97" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E97" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F97" s="17">
         <v>45064</v>
       </c>
       <c r="G97" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="H97" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="I97" s="23" t="s">
         <v>481</v>
-      </c>
-      <c r="H97" s="18" t="s">
-        <v>482</v>
-      </c>
-      <c r="I97" s="23" t="s">
-        <v>483</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>76</v>
@@ -7020,13 +7067,13 @@
         <v>76</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O97" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P97" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q97" s="2"/>
       <c r="R97" s="20"/>
@@ -7046,22 +7093,22 @@
         <v>27</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F98" s="17">
         <v>45064</v>
       </c>
       <c r="G98" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="H98" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="I98" s="23" t="s">
         <v>484</v>
-      </c>
-      <c r="H98" s="18" t="s">
-        <v>485</v>
-      </c>
-      <c r="I98" s="23" t="s">
-        <v>486</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>76</v>
@@ -7074,13 +7121,13 @@
         <v>76</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O98" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P98" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q98" s="2"/>
       <c r="R98" s="20"/>
@@ -7100,22 +7147,22 @@
         <v>27</v>
       </c>
       <c r="D99" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E99" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F99" s="17">
         <v>45064</v>
       </c>
       <c r="G99" s="18" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H99" s="18" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I99" s="23" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>76</v>
@@ -7128,13 +7175,13 @@
         <v>76</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O99" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P99" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q99" s="2"/>
       <c r="R99" s="20"/>
@@ -7154,22 +7201,22 @@
         <v>27</v>
       </c>
       <c r="D100" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E100" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F100" s="17">
         <v>45064</v>
       </c>
       <c r="G100" s="18" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H100" s="18" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I100" s="23" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>76</v>
@@ -7182,13 +7229,13 @@
         <v>76</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O100" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P100" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q100" s="2"/>
       <c r="R100" s="20"/>
@@ -7208,22 +7255,22 @@
         <v>27</v>
       </c>
       <c r="D101" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E101" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F101" s="17">
         <v>45064</v>
       </c>
       <c r="G101" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="H101" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="I101" s="23" t="s">
         <v>493</v>
-      </c>
-      <c r="H101" s="18" t="s">
-        <v>494</v>
-      </c>
-      <c r="I101" s="23" t="s">
-        <v>495</v>
       </c>
       <c r="J101" s="2" t="s">
         <v>76</v>
@@ -7236,13 +7283,13 @@
         <v>76</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O101" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P101" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q101" s="2"/>
       <c r="R101" s="20"/>
@@ -7262,22 +7309,22 @@
         <v>27</v>
       </c>
       <c r="D102" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E102" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F102" s="17">
         <v>45064</v>
       </c>
       <c r="G102" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="H102" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="I102" s="23" t="s">
         <v>496</v>
-      </c>
-      <c r="H102" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="I102" s="23" t="s">
-        <v>498</v>
       </c>
       <c r="J102" s="2" t="s">
         <v>76</v>
@@ -7290,13 +7337,13 @@
         <v>76</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O102" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P102" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q102" s="2"/>
       <c r="R102" s="20"/>
@@ -7316,22 +7363,22 @@
         <v>27</v>
       </c>
       <c r="D103" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E103" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F103" s="17">
         <v>45064</v>
       </c>
       <c r="G103" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="H103" s="18" t="s">
+        <v>498</v>
+      </c>
+      <c r="I103" s="23" t="s">
         <v>499</v>
-      </c>
-      <c r="H103" s="18" t="s">
-        <v>500</v>
-      </c>
-      <c r="I103" s="23" t="s">
-        <v>501</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>76</v>
@@ -7344,13 +7391,13 @@
         <v>76</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O103" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P103" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q103" s="2"/>
       <c r="R103" s="20"/>
@@ -7370,22 +7417,22 @@
         <v>27</v>
       </c>
       <c r="D104" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E104" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F104" s="17">
         <v>45065</v>
       </c>
       <c r="G104" s="18" t="s">
+        <v>503</v>
+      </c>
+      <c r="H104" s="18" t="s">
+        <v>504</v>
+      </c>
+      <c r="I104" s="23" t="s">
         <v>505</v>
-      </c>
-      <c r="H104" s="18" t="s">
-        <v>506</v>
-      </c>
-      <c r="I104" s="23" t="s">
-        <v>507</v>
       </c>
       <c r="J104" s="2" t="s">
         <v>76</v>
@@ -7398,13 +7445,13 @@
         <v>76</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O104" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P104" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q104" s="2"/>
       <c r="R104" s="20"/>
@@ -7424,22 +7471,22 @@
         <v>27</v>
       </c>
       <c r="D105" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E105" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F105" s="17">
         <v>45065</v>
       </c>
       <c r="G105" s="18" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H105" s="18" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I105" s="23" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="J105" s="2" t="s">
         <v>76</v>
@@ -7452,13 +7499,13 @@
         <v>76</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O105" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P105" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q105" s="2"/>
       <c r="R105" s="20"/>
@@ -7478,22 +7525,22 @@
         <v>27</v>
       </c>
       <c r="D106" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E106" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F106" s="17">
         <v>45065</v>
       </c>
       <c r="G106" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="H106" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="I106" s="23" t="s">
         <v>511</v>
-      </c>
-      <c r="H106" s="18" t="s">
-        <v>512</v>
-      </c>
-      <c r="I106" s="23" t="s">
-        <v>513</v>
       </c>
       <c r="J106" s="2" t="s">
         <v>76</v>
@@ -7506,13 +7553,13 @@
         <v>76</v>
       </c>
       <c r="N106" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O106" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P106" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q106" s="2"/>
       <c r="R106" s="20"/>
@@ -7532,22 +7579,22 @@
         <v>27</v>
       </c>
       <c r="D107" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E107" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F107" s="17">
         <v>45065</v>
       </c>
       <c r="G107" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="H107" s="18" t="s">
+        <v>501</v>
+      </c>
+      <c r="I107" s="23" t="s">
         <v>502</v>
-      </c>
-      <c r="H107" s="18" t="s">
-        <v>503</v>
-      </c>
-      <c r="I107" s="23" t="s">
-        <v>504</v>
       </c>
       <c r="J107" s="2" t="s">
         <v>76</v>
@@ -7560,13 +7607,13 @@
         <v>76</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O107" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P107" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q107" s="2"/>
       <c r="R107" s="20"/>
@@ -7586,22 +7633,22 @@
         <v>27</v>
       </c>
       <c r="D108" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F108" s="17">
         <v>45065</v>
       </c>
       <c r="G108" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="H108" s="18" t="s">
+        <v>513</v>
+      </c>
+      <c r="I108" s="23" t="s">
         <v>514</v>
-      </c>
-      <c r="H108" s="18" t="s">
-        <v>515</v>
-      </c>
-      <c r="I108" s="23" t="s">
-        <v>516</v>
       </c>
       <c r="J108" s="2" t="s">
         <v>76</v>
@@ -7614,13 +7661,13 @@
         <v>76</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O108" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P108" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q108" s="2"/>
       <c r="R108" s="20"/>
@@ -7629,7 +7676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="14">
         <v>147</v>
       </c>
@@ -7640,22 +7687,20 @@
         <v>28</v>
       </c>
       <c r="D109" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="E109" s="16" t="s">
-        <v>182</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="E109" s="16"/>
       <c r="F109" s="17">
         <v>45062</v>
       </c>
       <c r="G109" s="18" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H109" s="18" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I109" s="19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J109" s="2" t="s">
         <v>76</v>
@@ -7673,7 +7718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="14">
         <v>148</v>
       </c>
@@ -7684,22 +7729,20 @@
         <v>28</v>
       </c>
       <c r="D110" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>182</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="E110" s="16"/>
       <c r="F110" s="17">
         <v>45062</v>
       </c>
       <c r="G110" s="18" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H110" s="18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I110" s="19" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J110" s="2" t="s">
         <v>76</v>
@@ -7717,7 +7760,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="14">
         <v>149</v>
       </c>
@@ -7728,22 +7771,20 @@
         <v>28</v>
       </c>
       <c r="D111" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="E111" s="16" t="s">
-        <v>182</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="E111" s="16"/>
       <c r="F111" s="17">
         <v>45062</v>
       </c>
       <c r="G111" s="18" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H111" s="18" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I111" s="19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J111" s="2" t="s">
         <v>76</v>
@@ -7761,7 +7802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="14">
         <v>150</v>
       </c>
@@ -7772,22 +7813,20 @@
         <v>28</v>
       </c>
       <c r="D112" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="E112" s="16" t="s">
-        <v>182</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="E112" s="16"/>
       <c r="F112" s="17">
         <v>45062</v>
       </c>
       <c r="G112" s="18" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H112" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I112" s="19" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J112" s="2" t="s">
         <v>76</v>
@@ -7816,22 +7855,22 @@
         <v>28</v>
       </c>
       <c r="D113" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E113" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F113" s="17">
         <v>45062</v>
       </c>
       <c r="G113" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="H113" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="H113" s="18" t="s">
-        <v>333</v>
-      </c>
       <c r="I113" s="19" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="J113" s="2" t="s">
         <v>76</v>
@@ -7844,13 +7883,13 @@
         <v>76</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O113" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P113" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q113" s="2"/>
       <c r="R113" s="20"/>
@@ -7870,22 +7909,22 @@
         <v>28</v>
       </c>
       <c r="D114" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E114" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F114" s="17">
         <v>45062</v>
       </c>
       <c r="G114" s="18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H114" s="18" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I114" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J114" s="2" t="s">
         <v>76</v>
@@ -7898,13 +7937,13 @@
         <v>76</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O114" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P114" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q114" s="2"/>
       <c r="R114" s="20"/>
@@ -7924,22 +7963,22 @@
         <v>28</v>
       </c>
       <c r="D115" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E115" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F115" s="17">
         <v>45062</v>
       </c>
       <c r="G115" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="H115" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="I115" s="19" t="s">
         <v>337</v>
-      </c>
-      <c r="H115" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="I115" s="19" t="s">
-        <v>339</v>
       </c>
       <c r="J115" s="2" t="s">
         <v>76</v>
@@ -7952,13 +7991,13 @@
         <v>76</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O115" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P115" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q115" s="2"/>
       <c r="R115" s="20"/>
@@ -7978,22 +8017,22 @@
         <v>28</v>
       </c>
       <c r="D116" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E116" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F116" s="17">
         <v>45062</v>
       </c>
       <c r="G116" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="H116" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="I116" s="19" t="s">
         <v>340</v>
-      </c>
-      <c r="H116" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="I116" s="19" t="s">
-        <v>342</v>
       </c>
       <c r="J116" s="2" t="s">
         <v>76</v>
@@ -8006,13 +8045,13 @@
         <v>76</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O116" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P116" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q116" s="2"/>
       <c r="R116" s="20"/>
@@ -8032,22 +8071,22 @@
         <v>28</v>
       </c>
       <c r="D117" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E117" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F117" s="17">
         <v>45062</v>
       </c>
       <c r="G117" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="H117" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="I117" s="19" t="s">
         <v>343</v>
-      </c>
-      <c r="H117" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="I117" s="19" t="s">
-        <v>345</v>
       </c>
       <c r="J117" s="2" t="s">
         <v>76</v>
@@ -8060,13 +8099,13 @@
         <v>76</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O117" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P117" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q117" s="2"/>
       <c r="R117" s="20"/>
@@ -8086,22 +8125,22 @@
         <v>28</v>
       </c>
       <c r="D118" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E118" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F118" s="17">
         <v>45062</v>
       </c>
       <c r="G118" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="H118" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="I118" s="19" t="s">
         <v>346</v>
-      </c>
-      <c r="H118" s="18" t="s">
-        <v>347</v>
-      </c>
-      <c r="I118" s="19" t="s">
-        <v>348</v>
       </c>
       <c r="J118" s="2" t="s">
         <v>76</v>
@@ -8114,13 +8153,13 @@
         <v>76</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O118" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P118" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q118" s="2"/>
       <c r="R118" s="20"/>
@@ -8140,22 +8179,22 @@
         <v>28</v>
       </c>
       <c r="D119" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E119" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F119" s="17">
         <v>45062</v>
       </c>
       <c r="G119" s="18" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H119" s="18" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I119" s="19" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="J119" s="2" t="s">
         <v>76</v>
@@ -8168,13 +8207,13 @@
         <v>76</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O119" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P119" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q119" s="2"/>
       <c r="R119" s="20"/>
@@ -8194,22 +8233,22 @@
         <v>28</v>
       </c>
       <c r="D120" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E120" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F120" s="17">
         <v>45062</v>
       </c>
       <c r="G120" s="18" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H120" s="18" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I120" s="19" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J120" s="2" t="s">
         <v>76</v>
@@ -8222,13 +8261,13 @@
         <v>76</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O120" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P120" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q120" s="2"/>
       <c r="R120" s="20"/>
@@ -8248,22 +8287,22 @@
         <v>28</v>
       </c>
       <c r="D121" s="15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E121" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F121" s="17">
         <v>45062</v>
       </c>
       <c r="G121" s="18" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H121" s="18" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I121" s="19" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J121" s="2" t="s">
         <v>76</v>
@@ -8276,13 +8315,13 @@
         <v>76</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O121" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P121" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q121" s="2"/>
       <c r="R121" s="20"/>
@@ -8302,22 +8341,22 @@
         <v>28</v>
       </c>
       <c r="D122" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E122" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F122" s="17">
         <v>45063</v>
       </c>
       <c r="G122" s="18" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H122" s="18" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I122" s="19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J122" s="2" t="s">
         <v>76</v>
@@ -8330,13 +8369,13 @@
         <v>76</v>
       </c>
       <c r="N122" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O122" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P122" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q122" s="2"/>
       <c r="R122" s="20"/>
@@ -8356,22 +8395,22 @@
         <v>28</v>
       </c>
       <c r="D123" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E123" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F123" s="17">
         <v>45063</v>
       </c>
       <c r="G123" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="H123" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="I123" s="19" t="s">
         <v>359</v>
-      </c>
-      <c r="H123" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="I123" s="19" t="s">
-        <v>361</v>
       </c>
       <c r="J123" s="2" t="s">
         <v>76</v>
@@ -8384,13 +8423,13 @@
         <v>76</v>
       </c>
       <c r="N123" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O123" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P123" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q123" s="2"/>
       <c r="R123" s="20"/>
@@ -8410,22 +8449,22 @@
         <v>28</v>
       </c>
       <c r="D124" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E124" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F124" s="17">
         <v>45063</v>
       </c>
       <c r="G124" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="H124" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="I124" s="19" t="s">
         <v>364</v>
-      </c>
-      <c r="H124" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="I124" s="19" t="s">
-        <v>366</v>
       </c>
       <c r="J124" s="2" t="s">
         <v>76</v>
@@ -8438,13 +8477,13 @@
         <v>76</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O124" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P124" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q124" s="2"/>
       <c r="R124" s="20"/>
@@ -8464,22 +8503,22 @@
         <v>28</v>
       </c>
       <c r="D125" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E125" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F125" s="17">
         <v>45063</v>
       </c>
       <c r="G125" s="18" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H125" s="18" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I125" s="19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J125" s="2" t="s">
         <v>76</v>
@@ -8492,13 +8531,13 @@
         <v>76</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O125" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P125" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q125" s="2"/>
       <c r="R125" s="20"/>
@@ -8518,20 +8557,20 @@
         <v>28</v>
       </c>
       <c r="D126" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E126" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F126" s="17"/>
       <c r="G126" s="18"/>
       <c r="H126" s="18"/>
       <c r="I126" s="19"/>
       <c r="J126" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L126" s="2"/>
       <c r="M126" s="2"/>
@@ -8556,20 +8595,20 @@
         <v>28</v>
       </c>
       <c r="D127" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E127" s="16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F127" s="17"/>
       <c r="G127" s="18"/>
       <c r="H127" s="18"/>
       <c r="I127" s="19"/>
       <c r="J127" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L127" s="2"/>
       <c r="M127" s="2"/>
@@ -8594,20 +8633,20 @@
         <v>28</v>
       </c>
       <c r="D128" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E128" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F128" s="17"/>
       <c r="G128" s="18"/>
       <c r="H128" s="18"/>
       <c r="I128" s="19"/>
       <c r="J128" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L128" s="2"/>
       <c r="M128" s="2"/>
@@ -8632,20 +8671,20 @@
         <v>28</v>
       </c>
       <c r="D129" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E129" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F129" s="17"/>
       <c r="G129" s="18"/>
       <c r="H129" s="18"/>
       <c r="I129" s="19"/>
       <c r="J129" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K129" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L129" s="2"/>
       <c r="M129" s="2"/>
@@ -8670,29 +8709,27 @@
         <v>28</v>
       </c>
       <c r="D130" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E130" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F130" s="17">
         <v>45063</v>
       </c>
       <c r="G130" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="H130" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="I130" s="19" t="s">
         <v>372</v>
       </c>
-      <c r="H130" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="I130" s="19" t="s">
-        <v>374</v>
-      </c>
       <c r="J130" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K130" s="2" t="s">
-        <v>248</v>
-      </c>
+      <c r="K130" s="2"/>
       <c r="L130" s="2" t="s">
         <v>76</v>
       </c>
@@ -8700,13 +8737,13 @@
         <v>76</v>
       </c>
       <c r="N130" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O130" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P130" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q130" s="2"/>
       <c r="R130" s="20"/>
@@ -8726,26 +8763,26 @@
         <v>28</v>
       </c>
       <c r="D131" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E131" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F131" s="17"/>
       <c r="G131" s="18"/>
       <c r="H131" s="18"/>
       <c r="I131" s="19"/>
       <c r="J131" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K131" s="24" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L131" s="2"/>
       <c r="M131" s="2"/>
       <c r="N131" s="24"/>
       <c r="O131" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P131" s="2"/>
       <c r="Q131" s="2"/>
@@ -17962,6 +17999,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T131" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="19">
+      <filters>
+        <filter val="KO"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:T131">
       <sortCondition ref="A9:A131"/>
     </sortState>
@@ -18004,7 +18046,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
@@ -18012,10 +18054,10 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
File Json e reportChe
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DTSCONSULTI/DTSCONSULTINGSRL/DTSHIS/1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111DTSCONSULTI/DTSCONSULTINGSRL/DTSHIS/1.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc utente\Desktop\GATEWAY\S1#111DTSCONSULTI\DTSCONSULTINGSRL\DTSHIS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0562B125-1FDC-497B-93AE-C4A4A2392440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90CFA66-1973-4ECA-B36E-0152573770C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -832,13 +832,7 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.2e536b3745^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-05-11T17:26:25Z</t>
-  </si>
-  <si>
     <t>ef8bbca283018805</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.502517a585^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>2023-05-11T17:36:52Z</t>
@@ -1100,37 +1094,10 @@
     <t>2023-05-16T16:56:37Z</t>
   </si>
   <si>
-    <t>2023-05-16T16:56:40Z</t>
-  </si>
-  <si>
-    <t>2023-05-16T16:56:41Z</t>
-  </si>
-  <si>
-    <t>2023-05-16T16:56:43Z</t>
-  </si>
-  <si>
     <t>72e253b18215dc79</t>
   </si>
   <si>
-    <t>4a52844aceab70d1</t>
-  </si>
-  <si>
-    <t>b8d9794b5ef6ecf0</t>
-  </si>
-  <si>
-    <t>fec09f05dc2009e1</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.26d953da18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.d6552f21e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.d19803891f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.ac59c29294^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <r>
@@ -1522,39 +1489,21 @@
     <t>9aeeca273e560a18</t>
   </si>
   <si>
-    <t>2023-05-17T15:33:16Z</t>
-  </si>
-  <si>
     <t>2023-05-17T15:33:31Z</t>
   </si>
   <si>
-    <t>2023-05-17T15:42:42Z</t>
-  </si>
-  <si>
     <t>2023-05-17T15:43:49Z</t>
   </si>
   <si>
     <t>617fda1f37045bbb</t>
   </si>
   <si>
-    <t>9da6d0a39844a16f</t>
-  </si>
-  <si>
     <t>31a9ec494be84b04</t>
   </si>
   <si>
-    <t>b330f71ef5ebcf23</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.21d1ef3f59^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.6a0704ecfd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.1bdeb0e2d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.e07291d0e9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -1817,6 +1766,57 @@
   </si>
   <si>
     <t>l programma nella Form presidiata mostra un messaggio a video con l'errore che proviene dal servizio</t>
+  </si>
+  <si>
+    <t>7ef685830355d2ed</t>
+  </si>
+  <si>
+    <t>2023-06-09T14:56:16Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.4f93d3b444^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.4aad8a788c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>47a2d75b3ba5673d</t>
+  </si>
+  <si>
+    <t>2023-06-09T14:59:42Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.73edf2fd9b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-09T15:26:25Z</t>
+  </si>
+  <si>
+    <t>8c28240b6d3c06c9</t>
+  </si>
+  <si>
+    <t>2023-06-09T18:20:40Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.1803f2626d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a645b0a2a1c3b61f</t>
+  </si>
+  <si>
+    <t>2023-06-09T18:21:40Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.d8eb0b0c9f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9dee1b038c62ae5d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.6e01010233^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-09T18:22:40Z</t>
   </si>
 </sst>
 </file>
@@ -2170,6 +2170,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2192,12 +2198,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2492,14 +2492,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T726"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="J33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P37" sqref="P37"/>
+      <selection pane="bottomRight" activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="91.7109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2546,14 +2545,14 @@
       <c r="T1" s="9"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="33"/>
+      <c r="D2" s="35"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -2571,14 +2570,14 @@
       <c r="T2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="40" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="33"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -2596,12 +2595,12 @@
       <c r="T3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="40" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -2620,12 +2619,12 @@
       <c r="T4" s="9"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="33"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -2643,8 +2642,8 @@
       <c r="T5" s="9"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="10"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -2761,7 +2760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>1</v>
       </c>
@@ -2805,7 +2804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>2</v>
       </c>
@@ -2849,7 +2848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>3</v>
       </c>
@@ -2893,7 +2892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>4</v>
       </c>
@@ -2910,16 +2909,16 @@
         <v>37</v>
       </c>
       <c r="F13" s="17">
-        <v>45057</v>
+        <v>45086</v>
       </c>
       <c r="G13" s="18" t="s">
+        <v>517</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>228</v>
-      </c>
       <c r="I13" s="19" t="s">
-        <v>229</v>
+        <v>516</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>76</v>
@@ -2937,7 +2936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>5</v>
       </c>
@@ -2957,13 +2956,13 @@
         <v>45057</v>
       </c>
       <c r="G14" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="I14" s="19" t="s">
         <v>230</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>76</v>
@@ -2981,7 +2980,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>6</v>
       </c>
@@ -3001,13 +3000,13 @@
         <v>45063</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>76</v>
@@ -3025,7 +3024,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>7</v>
       </c>
@@ -3045,13 +3044,13 @@
         <v>45063</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>76</v>
@@ -3069,7 +3068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
         <v>8</v>
       </c>
@@ -3089,13 +3088,13 @@
         <v>45063</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>76</v>
@@ -3113,7 +3112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>9</v>
       </c>
@@ -3133,13 +3132,13 @@
         <v>45063</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>76</v>
@@ -3157,7 +3156,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>11</v>
       </c>
@@ -3177,13 +3176,13 @@
         <v>45062</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>76</v>
@@ -3201,7 +3200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
         <v>12</v>
       </c>
@@ -3221,13 +3220,13 @@
         <v>45062</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>76</v>
@@ -3245,7 +3244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>13</v>
       </c>
@@ -3269,7 +3268,7 @@
         <v>213</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -3283,7 +3282,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <v>14</v>
       </c>
@@ -3307,7 +3306,7 @@
         <v>213</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -3321,7 +3320,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>24</v>
       </c>
@@ -3338,16 +3337,16 @@
         <v>57</v>
       </c>
       <c r="F23" s="17">
-        <v>45063</v>
+        <v>45086</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>428</v>
+        <v>511</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>435</v>
+        <v>510</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>436</v>
+        <v>512</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>76</v>
@@ -3365,7 +3364,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <v>25</v>
       </c>
@@ -3385,13 +3384,13 @@
         <v>45063</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>76</v>
@@ -3409,7 +3408,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
         <v>26</v>
       </c>
@@ -3426,16 +3425,16 @@
         <v>61</v>
       </c>
       <c r="F25" s="17">
-        <v>45063</v>
+        <v>45086</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>430</v>
+        <v>515</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>433</v>
+        <v>514</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>438</v>
+        <v>513</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>76</v>
@@ -3453,7 +3452,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>27</v>
       </c>
@@ -3473,13 +3472,13 @@
         <v>45063</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>76</v>
@@ -3511,7 +3510,7 @@
         <v>64</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
@@ -3521,14 +3520,14 @@
         <v>213</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="20"/>
@@ -3551,7 +3550,7 @@
         <v>65</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
@@ -3561,14 +3560,14 @@
         <v>213</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="20"/>
@@ -3591,7 +3590,7 @@
         <v>66</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
@@ -3601,14 +3600,14 @@
         <v>213</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="20"/>
@@ -3631,7 +3630,7 @@
         <v>67</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
@@ -3641,14 +3640,14 @@
         <v>213</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="20"/>
@@ -3671,7 +3670,7 @@
         <v>68</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="18"/>
@@ -3681,14 +3680,14 @@
         <v>213</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="20"/>
@@ -3711,19 +3710,19 @@
         <v>69</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F32" s="17">
         <v>45062</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>76</v>
@@ -3736,13 +3735,13 @@
         <v>76</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="20"/>
@@ -3765,19 +3764,19 @@
         <v>70</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F33" s="17">
         <v>45063</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>76</v>
@@ -3790,13 +3789,13 @@
         <v>76</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="20"/>
@@ -3819,22 +3818,22 @@
         <v>71</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F34" s="17">
         <v>45062</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
@@ -3844,13 +3843,13 @@
         <v>76</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O34" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="20"/>
@@ -3873,19 +3872,19 @@
         <v>72</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F35" s="17">
         <v>45062</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>76</v>
@@ -3898,13 +3897,13 @@
         <v>76</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O35" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="20"/>
@@ -3927,19 +3926,19 @@
         <v>73</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F36" s="17">
         <v>45063</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>76</v>
@@ -3952,13 +3951,13 @@
         <v>76</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O36" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="20"/>
@@ -3994,15 +3993,15 @@
       <c r="L37" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M37" s="42" t="s">
+      <c r="M37" s="29" t="s">
         <v>76</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
       <c r="O37" s="2"/>
-      <c r="P37" s="41" t="s">
-        <v>525</v>
+      <c r="P37" s="28" t="s">
+        <v>508</v>
       </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="20"/>
@@ -4038,7 +4037,7 @@
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="20" t="s">
@@ -4076,7 +4075,7 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Q39" s="2"/>
       <c r="R39" s="20" t="s">
@@ -4114,7 +4113,7 @@
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Q40" s="2"/>
       <c r="R40" s="20" t="s">
@@ -4152,7 +4151,7 @@
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="20" t="s">
@@ -4183,13 +4182,13 @@
         <v>45062</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>76</v>
@@ -4202,13 +4201,13 @@
         <v>76</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="20"/>
@@ -4237,13 +4236,13 @@
         <v>45062</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>76</v>
@@ -4256,13 +4255,13 @@
         <v>76</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O43" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="20"/>
@@ -4291,13 +4290,13 @@
         <v>45062</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>515</v>
+        <v>498</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>76</v>
@@ -4310,13 +4309,13 @@
         <v>76</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O44" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q44" s="2"/>
       <c r="R44" s="20"/>
@@ -4345,13 +4344,13 @@
         <v>45062</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>76</v>
@@ -4364,13 +4363,13 @@
         <v>76</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O45" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="20"/>
@@ -4399,13 +4398,13 @@
         <v>45072</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>517</v>
+        <v>500</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>76</v>
@@ -4418,13 +4417,13 @@
         <v>76</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q46" s="2"/>
       <c r="R46" s="20"/>
@@ -4453,13 +4452,13 @@
         <v>45062</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I47" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>76</v>
@@ -4472,13 +4471,13 @@
         <v>76</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O47" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="20"/>
@@ -4507,13 +4506,13 @@
         <v>45062</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>76</v>
@@ -4526,13 +4525,13 @@
         <v>76</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q48" s="2"/>
       <c r="R48" s="20"/>
@@ -4561,13 +4560,13 @@
         <v>45072</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>521</v>
+        <v>504</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>520</v>
+        <v>503</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>519</v>
+        <v>502</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>76</v>
@@ -4580,13 +4579,13 @@
         <v>76</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q49" s="2"/>
       <c r="R49" s="20"/>
@@ -4615,13 +4614,13 @@
         <v>45062</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>76</v>
@@ -4634,13 +4633,13 @@
         <v>76</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q50" s="2"/>
       <c r="R50" s="20"/>
@@ -4669,13 +4668,13 @@
         <v>45062</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>76</v>
@@ -4688,13 +4687,13 @@
         <v>76</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O51" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q51" s="2"/>
       <c r="R51" s="20"/>
@@ -4723,13 +4722,13 @@
         <v>45072</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>522</v>
+        <v>505</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>76</v>
@@ -4742,13 +4741,13 @@
         <v>76</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O52" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q52" s="2"/>
       <c r="R52" s="20"/>
@@ -4777,13 +4776,13 @@
         <v>45063</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>76</v>
@@ -4796,13 +4795,13 @@
         <v>76</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O53" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q53" s="2"/>
       <c r="R53" s="20"/>
@@ -4831,13 +4830,13 @@
         <v>45063</v>
       </c>
       <c r="G54" s="18" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>76</v>
@@ -4850,13 +4849,13 @@
         <v>76</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O54" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q54" s="2"/>
       <c r="R54" s="20"/>
@@ -4885,13 +4884,13 @@
         <v>45063</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>76</v>
@@ -4904,13 +4903,13 @@
         <v>76</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q55" s="2"/>
       <c r="R55" s="20"/>
@@ -4939,13 +4938,13 @@
         <v>45063</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>76</v>
@@ -4958,13 +4957,13 @@
         <v>76</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" s="20"/>
@@ -4993,13 +4992,13 @@
         <v>45063</v>
       </c>
       <c r="G57" s="18" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>76</v>
@@ -5012,13 +5011,13 @@
         <v>76</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q57" s="2"/>
       <c r="R57" s="20"/>
@@ -5047,13 +5046,13 @@
         <v>45063</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="H58" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="I58" s="23" t="s">
         <v>408</v>
-      </c>
-      <c r="I58" s="23" t="s">
-        <v>419</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>76</v>
@@ -5066,13 +5065,13 @@
         <v>76</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O58" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" s="20"/>
@@ -5101,13 +5100,13 @@
         <v>45063</v>
       </c>
       <c r="G59" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="H59" s="18" t="s">
         <v>396</v>
       </c>
-      <c r="H59" s="18" t="s">
-        <v>407</v>
-      </c>
       <c r="I59" s="23" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>76</v>
@@ -5120,13 +5119,13 @@
         <v>76</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="20"/>
@@ -5155,13 +5154,13 @@
         <v>45063</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>76</v>
@@ -5174,13 +5173,13 @@
         <v>76</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O60" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="20"/>
@@ -5209,13 +5208,13 @@
         <v>45063</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>76</v>
@@ -5228,13 +5227,13 @@
         <v>76</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P61" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="20"/>
@@ -5263,13 +5262,13 @@
         <v>45063</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>76</v>
@@ -5282,13 +5281,13 @@
         <v>76</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O62" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="20"/>
@@ -5317,13 +5316,13 @@
         <v>45063</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>76</v>
@@ -5336,13 +5335,13 @@
         <v>76</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O63" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q63" s="2"/>
       <c r="R63" s="20"/>
@@ -5371,13 +5370,13 @@
         <v>45063</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>76</v>
@@ -5390,13 +5389,13 @@
         <v>76</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O64" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q64" s="2"/>
       <c r="R64" s="20"/>
@@ -5425,13 +5424,13 @@
         <v>45062</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>76</v>
@@ -5444,13 +5443,13 @@
         <v>76</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O65" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P65" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q65" s="2"/>
       <c r="R65" s="20"/>
@@ -5479,13 +5478,13 @@
         <v>45062</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>76</v>
@@ -5498,13 +5497,13 @@
         <v>76</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O66" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q66" s="2"/>
       <c r="R66" s="20"/>
@@ -5533,13 +5532,13 @@
         <v>45062</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>76</v>
@@ -5552,13 +5551,13 @@
         <v>76</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O67" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q67" s="2"/>
       <c r="R67" s="20"/>
@@ -5587,13 +5586,13 @@
         <v>45062</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I68" s="23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>76</v>
@@ -5606,13 +5605,13 @@
         <v>76</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O68" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P68" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="20"/>
@@ -5641,13 +5640,13 @@
         <v>45062</v>
       </c>
       <c r="G69" s="18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I69" s="23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>76</v>
@@ -5660,13 +5659,13 @@
         <v>76</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O69" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P69" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="20"/>
@@ -5695,13 +5694,13 @@
         <v>45062</v>
       </c>
       <c r="G70" s="18" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I70" s="23" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>76</v>
@@ -5714,13 +5713,13 @@
         <v>76</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O70" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="20"/>
@@ -5749,13 +5748,13 @@
         <v>45062</v>
       </c>
       <c r="G71" s="18" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I71" s="23" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>76</v>
@@ -5768,13 +5767,13 @@
         <v>76</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O71" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q71" s="2"/>
       <c r="R71" s="20"/>
@@ -5803,13 +5802,13 @@
         <v>45062</v>
       </c>
       <c r="G72" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I72" s="23" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>76</v>
@@ -5822,13 +5821,13 @@
         <v>76</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O72" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P72" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q72" s="2"/>
       <c r="R72" s="20"/>
@@ -5857,13 +5856,13 @@
         <v>45062</v>
       </c>
       <c r="G73" s="18" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I73" s="23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>76</v>
@@ -5876,13 +5875,13 @@
         <v>76</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O73" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P73" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q73" s="2"/>
       <c r="R73" s="20"/>
@@ -5911,13 +5910,13 @@
         <v>45062</v>
       </c>
       <c r="G74" s="18" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H74" s="18" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I74" s="23" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>76</v>
@@ -5930,13 +5929,13 @@
         <v>76</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O74" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P74" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q74" s="2"/>
       <c r="R74" s="20"/>
@@ -5965,13 +5964,13 @@
         <v>45062</v>
       </c>
       <c r="G75" s="18" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I75" s="23" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>76</v>
@@ -5984,13 +5983,13 @@
         <v>76</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O75" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q75" s="2"/>
       <c r="R75" s="20"/>
@@ -6019,13 +6018,13 @@
         <v>45062</v>
       </c>
       <c r="G76" s="18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H76" s="18" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I76" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>76</v>
@@ -6038,13 +6037,13 @@
         <v>76</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O76" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q76" s="2"/>
       <c r="R76" s="20"/>
@@ -6077,12 +6076,12 @@
         <v>213</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
@@ -6117,12 +6116,12 @@
         <v>213</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
@@ -6157,12 +6156,12 @@
         <v>213</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
@@ -6197,12 +6196,12 @@
         <v>213</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
       <c r="N80" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
@@ -6237,12 +6236,12 @@
         <v>213</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
@@ -6273,13 +6272,13 @@
         <v>45062</v>
       </c>
       <c r="G82" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="H82" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="I82" s="23" t="s">
         <v>311</v>
-      </c>
-      <c r="H82" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="I82" s="23" t="s">
-        <v>313</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>76</v>
@@ -6292,13 +6291,13 @@
         <v>76</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O82" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P82" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q82" s="2"/>
       <c r="R82" s="20"/>
@@ -6327,13 +6326,13 @@
         <v>45062</v>
       </c>
       <c r="G83" s="18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H83" s="18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I83" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>76</v>
@@ -6346,13 +6345,13 @@
         <v>76</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O83" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P83" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q83" s="2"/>
       <c r="R83" s="20"/>
@@ -6381,13 +6380,13 @@
         <v>45063</v>
       </c>
       <c r="G84" s="18" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
       <c r="H84" s="18" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
       <c r="I84" s="23" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>76</v>
@@ -6400,13 +6399,13 @@
         <v>76</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O84" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P84" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q84" s="2"/>
       <c r="R84" s="20"/>
@@ -6435,13 +6434,13 @@
         <v>45063</v>
       </c>
       <c r="G85" s="18" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
       <c r="H85" s="18" t="s">
-        <v>450</v>
+        <v>433</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>76</v>
@@ -6454,13 +6453,13 @@
         <v>76</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O85" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P85" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q85" s="2"/>
       <c r="R85" s="20"/>
@@ -6489,13 +6488,13 @@
         <v>45063</v>
       </c>
       <c r="G86" s="18" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="H86" s="18" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>454</v>
+        <v>437</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>76</v>
@@ -6508,13 +6507,13 @@
         <v>76</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O86" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P86" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q86" s="2"/>
       <c r="R86" s="20"/>
@@ -6543,13 +6542,13 @@
         <v>45063</v>
       </c>
       <c r="G87" s="18" t="s">
-        <v>443</v>
+        <v>426</v>
       </c>
       <c r="H87" s="18" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>455</v>
+        <v>438</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>76</v>
@@ -6562,13 +6561,13 @@
         <v>76</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O87" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P87" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q87" s="2"/>
       <c r="R87" s="20"/>
@@ -6597,13 +6596,13 @@
         <v>45063</v>
       </c>
       <c r="G88" s="18" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="H88" s="18" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
       <c r="I88" s="23" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>76</v>
@@ -6616,13 +6615,13 @@
         <v>76</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O88" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P88" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q88" s="2"/>
       <c r="R88" s="20"/>
@@ -6651,13 +6650,13 @@
         <v>45063</v>
       </c>
       <c r="G89" s="18" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
       <c r="H89" s="18" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
       <c r="I89" s="23" t="s">
-        <v>457</v>
+        <v>440</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>76</v>
@@ -6670,13 +6669,13 @@
         <v>76</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O89" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P89" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q89" s="2"/>
       <c r="R89" s="20"/>
@@ -6705,13 +6704,13 @@
         <v>45063</v>
       </c>
       <c r="G90" s="18" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="H90" s="18" t="s">
-        <v>458</v>
+        <v>441</v>
       </c>
       <c r="I90" s="23" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>76</v>
@@ -6724,13 +6723,13 @@
         <v>76</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q90" s="2"/>
       <c r="R90" s="20"/>
@@ -6759,13 +6758,13 @@
         <v>45064</v>
       </c>
       <c r="G91" s="18" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="H91" s="18" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="I91" s="23" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>76</v>
@@ -6778,13 +6777,13 @@
         <v>76</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O91" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P91" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q91" s="2"/>
       <c r="R91" s="20"/>
@@ -6813,13 +6812,13 @@
         <v>45064</v>
       </c>
       <c r="G92" s="18" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="H92" s="18" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="I92" s="23" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>76</v>
@@ -6832,13 +6831,13 @@
         <v>76</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O92" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q92" s="2"/>
       <c r="R92" s="20"/>
@@ -6867,13 +6866,13 @@
         <v>45064</v>
       </c>
       <c r="G93" s="18" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
       <c r="H93" s="18" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="I93" s="23" t="s">
-        <v>471</v>
+        <v>454</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>76</v>
@@ -6886,13 +6885,13 @@
         <v>76</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O93" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q93" s="2"/>
       <c r="R93" s="20"/>
@@ -6921,13 +6920,13 @@
         <v>45064</v>
       </c>
       <c r="G94" s="18" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
       <c r="H94" s="18" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="I94" s="23" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>76</v>
@@ -6940,13 +6939,13 @@
         <v>76</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O94" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P94" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q94" s="2"/>
       <c r="R94" s="20"/>
@@ -6975,13 +6974,13 @@
         <v>45064</v>
       </c>
       <c r="G95" s="18" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
       <c r="H95" s="18" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="I95" s="23" t="s">
-        <v>477</v>
+        <v>460</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>76</v>
@@ -6994,13 +6993,13 @@
         <v>76</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O95" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P95" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q95" s="2"/>
       <c r="R95" s="20"/>
@@ -7029,13 +7028,13 @@
         <v>45064</v>
       </c>
       <c r="G96" s="18" t="s">
-        <v>474</v>
+        <v>457</v>
       </c>
       <c r="H96" s="18" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="I96" s="23" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>76</v>
@@ -7048,13 +7047,13 @@
         <v>76</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O96" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P96" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q96" s="2"/>
       <c r="R96" s="20"/>
@@ -7083,13 +7082,13 @@
         <v>45064</v>
       </c>
       <c r="G97" s="18" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="H97" s="18" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="I97" s="23" t="s">
-        <v>481</v>
+        <v>464</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>76</v>
@@ -7102,13 +7101,13 @@
         <v>76</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O97" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P97" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q97" s="2"/>
       <c r="R97" s="20"/>
@@ -7137,13 +7136,13 @@
         <v>45064</v>
       </c>
       <c r="G98" s="18" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c r="H98" s="18" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
       <c r="I98" s="23" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>76</v>
@@ -7156,13 +7155,13 @@
         <v>76</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O98" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P98" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q98" s="2"/>
       <c r="R98" s="20"/>
@@ -7191,13 +7190,13 @@
         <v>45064</v>
       </c>
       <c r="G99" s="18" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
       <c r="H99" s="18" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
       <c r="I99" s="23" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>76</v>
@@ -7210,13 +7209,13 @@
         <v>76</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O99" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P99" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q99" s="2"/>
       <c r="R99" s="20"/>
@@ -7245,13 +7244,13 @@
         <v>45064</v>
       </c>
       <c r="G100" s="18" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
       <c r="H100" s="18" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="I100" s="23" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>76</v>
@@ -7264,13 +7263,13 @@
         <v>76</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O100" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P100" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q100" s="2"/>
       <c r="R100" s="20"/>
@@ -7299,13 +7298,13 @@
         <v>45064</v>
       </c>
       <c r="G101" s="18" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="H101" s="18" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="I101" s="23" t="s">
-        <v>493</v>
+        <v>476</v>
       </c>
       <c r="J101" s="2" t="s">
         <v>76</v>
@@ -7318,13 +7317,13 @@
         <v>76</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O101" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P101" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q101" s="2"/>
       <c r="R101" s="20"/>
@@ -7353,13 +7352,13 @@
         <v>45064</v>
       </c>
       <c r="G102" s="18" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
       <c r="H102" s="18" t="s">
-        <v>495</v>
+        <v>478</v>
       </c>
       <c r="I102" s="23" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
       <c r="J102" s="2" t="s">
         <v>76</v>
@@ -7372,13 +7371,13 @@
         <v>76</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O102" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P102" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q102" s="2"/>
       <c r="R102" s="20"/>
@@ -7407,13 +7406,13 @@
         <v>45064</v>
       </c>
       <c r="G103" s="18" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
       <c r="H103" s="18" t="s">
-        <v>498</v>
+        <v>481</v>
       </c>
       <c r="I103" s="23" t="s">
-        <v>499</v>
+        <v>482</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>76</v>
@@ -7426,13 +7425,13 @@
         <v>76</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O103" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P103" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q103" s="2"/>
       <c r="R103" s="20"/>
@@ -7461,13 +7460,13 @@
         <v>45065</v>
       </c>
       <c r="G104" s="18" t="s">
-        <v>503</v>
+        <v>486</v>
       </c>
       <c r="H104" s="18" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
       <c r="I104" s="23" t="s">
-        <v>505</v>
+        <v>488</v>
       </c>
       <c r="J104" s="2" t="s">
         <v>76</v>
@@ -7480,13 +7479,13 @@
         <v>76</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O104" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P104" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q104" s="2"/>
       <c r="R104" s="20"/>
@@ -7515,13 +7514,13 @@
         <v>45065</v>
       </c>
       <c r="G105" s="18" t="s">
-        <v>508</v>
+        <v>491</v>
       </c>
       <c r="H105" s="18" t="s">
-        <v>507</v>
+        <v>490</v>
       </c>
       <c r="I105" s="23" t="s">
-        <v>506</v>
+        <v>489</v>
       </c>
       <c r="J105" s="2" t="s">
         <v>76</v>
@@ -7534,13 +7533,13 @@
         <v>76</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O105" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P105" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q105" s="2"/>
       <c r="R105" s="20"/>
@@ -7569,13 +7568,13 @@
         <v>45065</v>
       </c>
       <c r="G106" s="18" t="s">
-        <v>509</v>
+        <v>492</v>
       </c>
       <c r="H106" s="18" t="s">
-        <v>510</v>
+        <v>493</v>
       </c>
       <c r="I106" s="23" t="s">
-        <v>511</v>
+        <v>494</v>
       </c>
       <c r="J106" s="2" t="s">
         <v>76</v>
@@ -7588,13 +7587,13 @@
         <v>76</v>
       </c>
       <c r="N106" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O106" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P106" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q106" s="2"/>
       <c r="R106" s="20"/>
@@ -7623,13 +7622,13 @@
         <v>45065</v>
       </c>
       <c r="G107" s="18" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
       <c r="H107" s="18" t="s">
-        <v>501</v>
+        <v>484</v>
       </c>
       <c r="I107" s="23" t="s">
-        <v>502</v>
+        <v>485</v>
       </c>
       <c r="J107" s="2" t="s">
         <v>76</v>
@@ -7642,13 +7641,13 @@
         <v>76</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O107" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P107" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q107" s="2"/>
       <c r="R107" s="20"/>
@@ -7677,13 +7676,13 @@
         <v>45065</v>
       </c>
       <c r="G108" s="18" t="s">
-        <v>512</v>
+        <v>495</v>
       </c>
       <c r="H108" s="18" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="I108" s="23" t="s">
-        <v>514</v>
+        <v>497</v>
       </c>
       <c r="J108" s="2" t="s">
         <v>76</v>
@@ -7696,13 +7695,13 @@
         <v>76</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O108" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P108" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q108" s="2"/>
       <c r="R108" s="20"/>
@@ -7711,7 +7710,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="14">
         <v>147</v>
       </c>
@@ -7729,13 +7728,13 @@
         <v>45062</v>
       </c>
       <c r="G109" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="H109" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="I109" s="19" t="s">
         <v>315</v>
-      </c>
-      <c r="H109" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="I109" s="19" t="s">
-        <v>323</v>
       </c>
       <c r="J109" s="2" t="s">
         <v>76</v>
@@ -7753,7 +7752,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="14">
         <v>148</v>
       </c>
@@ -7768,16 +7767,16 @@
       </c>
       <c r="E110" s="16"/>
       <c r="F110" s="17">
-        <v>45062</v>
+        <v>45086</v>
       </c>
       <c r="G110" s="18" t="s">
-        <v>316</v>
+        <v>519</v>
       </c>
       <c r="H110" s="18" t="s">
-        <v>320</v>
+        <v>518</v>
       </c>
       <c r="I110" s="19" t="s">
-        <v>324</v>
+        <v>520</v>
       </c>
       <c r="J110" s="2" t="s">
         <v>76</v>
@@ -7795,7 +7794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="14">
         <v>149</v>
       </c>
@@ -7810,16 +7809,16 @@
       </c>
       <c r="E111" s="16"/>
       <c r="F111" s="17">
-        <v>45062</v>
+        <v>45086</v>
       </c>
       <c r="G111" s="18" t="s">
-        <v>317</v>
+        <v>522</v>
       </c>
       <c r="H111" s="18" t="s">
-        <v>321</v>
+        <v>521</v>
       </c>
       <c r="I111" s="19" t="s">
-        <v>325</v>
+        <v>523</v>
       </c>
       <c r="J111" s="2" t="s">
         <v>76</v>
@@ -7837,7 +7836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="14">
         <v>150</v>
       </c>
@@ -7852,16 +7851,16 @@
       </c>
       <c r="E112" s="16"/>
       <c r="F112" s="17">
-        <v>45062</v>
+        <v>45086</v>
       </c>
       <c r="G112" s="18" t="s">
-        <v>318</v>
+        <v>526</v>
       </c>
       <c r="H112" s="18" t="s">
-        <v>322</v>
+        <v>524</v>
       </c>
       <c r="I112" s="19" t="s">
-        <v>326</v>
+        <v>525</v>
       </c>
       <c r="J112" s="2" t="s">
         <v>76</v>
@@ -7899,13 +7898,13 @@
         <v>45062</v>
       </c>
       <c r="G113" s="18" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="H113" s="18" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="I113" s="19" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="J113" s="2" t="s">
         <v>76</v>
@@ -7918,13 +7917,13 @@
         <v>76</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O113" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P113" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q113" s="2"/>
       <c r="R113" s="20"/>
@@ -7953,13 +7952,13 @@
         <v>45062</v>
       </c>
       <c r="G114" s="18" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="H114" s="18" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="I114" s="19" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="J114" s="2" t="s">
         <v>76</v>
@@ -7972,13 +7971,13 @@
         <v>76</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O114" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P114" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q114" s="2"/>
       <c r="R114" s="20"/>
@@ -8007,13 +8006,13 @@
         <v>45062</v>
       </c>
       <c r="G115" s="18" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="H115" s="18" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="I115" s="19" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="J115" s="2" t="s">
         <v>76</v>
@@ -8026,13 +8025,13 @@
         <v>76</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O115" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P115" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q115" s="2"/>
       <c r="R115" s="20"/>
@@ -8061,13 +8060,13 @@
         <v>45062</v>
       </c>
       <c r="G116" s="18" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="H116" s="18" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="I116" s="19" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="J116" s="2" t="s">
         <v>76</v>
@@ -8080,13 +8079,13 @@
         <v>76</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O116" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P116" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q116" s="2"/>
       <c r="R116" s="20"/>
@@ -8115,13 +8114,13 @@
         <v>45062</v>
       </c>
       <c r="G117" s="18" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="H117" s="18" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="I117" s="19" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="J117" s="2" t="s">
         <v>76</v>
@@ -8134,13 +8133,13 @@
         <v>76</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O117" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P117" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q117" s="2"/>
       <c r="R117" s="20"/>
@@ -8169,13 +8168,13 @@
         <v>45062</v>
       </c>
       <c r="G118" s="18" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="H118" s="18" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="I118" s="19" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="J118" s="2" t="s">
         <v>76</v>
@@ -8188,13 +8187,13 @@
         <v>76</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O118" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P118" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q118" s="2"/>
       <c r="R118" s="20"/>
@@ -8223,13 +8222,13 @@
         <v>45062</v>
       </c>
       <c r="G119" s="18" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="H119" s="18" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="I119" s="19" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="J119" s="2" t="s">
         <v>76</v>
@@ -8242,13 +8241,13 @@
         <v>76</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O119" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P119" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q119" s="2"/>
       <c r="R119" s="20"/>
@@ -8277,13 +8276,13 @@
         <v>45062</v>
       </c>
       <c r="G120" s="18" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="H120" s="18" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="I120" s="19" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="J120" s="2" t="s">
         <v>76</v>
@@ -8296,13 +8295,13 @@
         <v>76</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O120" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P120" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q120" s="2"/>
       <c r="R120" s="20"/>
@@ -8331,13 +8330,13 @@
         <v>45062</v>
       </c>
       <c r="G121" s="18" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="H121" s="18" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="I121" s="19" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="J121" s="2" t="s">
         <v>76</v>
@@ -8350,13 +8349,13 @@
         <v>76</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O121" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P121" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q121" s="2"/>
       <c r="R121" s="20"/>
@@ -8385,13 +8384,13 @@
         <v>45063</v>
       </c>
       <c r="G122" s="18" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="H122" s="18" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="I122" s="19" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="J122" s="2" t="s">
         <v>76</v>
@@ -8404,13 +8403,13 @@
         <v>76</v>
       </c>
       <c r="N122" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O122" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P122" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q122" s="2"/>
       <c r="R122" s="20"/>
@@ -8439,13 +8438,13 @@
         <v>45063</v>
       </c>
       <c r="G123" s="18" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="H123" s="18" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="I123" s="19" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="J123" s="2" t="s">
         <v>76</v>
@@ -8458,13 +8457,13 @@
         <v>76</v>
       </c>
       <c r="N123" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O123" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P123" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q123" s="2"/>
       <c r="R123" s="20"/>
@@ -8493,13 +8492,13 @@
         <v>45063</v>
       </c>
       <c r="G124" s="18" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="H124" s="18" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="I124" s="19" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="J124" s="2" t="s">
         <v>76</v>
@@ -8512,13 +8511,13 @@
         <v>76</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O124" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P124" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q124" s="2"/>
       <c r="R124" s="20"/>
@@ -8547,13 +8546,13 @@
         <v>45063</v>
       </c>
       <c r="G125" s="18" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="H125" s="18" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="I125" s="19" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="J125" s="2" t="s">
         <v>76</v>
@@ -8566,13 +8565,13 @@
         <v>76</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O125" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P125" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q125" s="2"/>
       <c r="R125" s="20"/>
@@ -8605,7 +8604,7 @@
         <v>213</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="L126" s="2"/>
       <c r="M126" s="2"/>
@@ -8643,7 +8642,7 @@
         <v>213</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="L127" s="2"/>
       <c r="M127" s="2"/>
@@ -8681,7 +8680,7 @@
         <v>213</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="L128" s="2"/>
       <c r="M128" s="2"/>
@@ -8719,7 +8718,7 @@
         <v>213</v>
       </c>
       <c r="K129" s="2" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="L129" s="2"/>
       <c r="M129" s="2"/>
@@ -8753,13 +8752,13 @@
         <v>45063</v>
       </c>
       <c r="G130" s="18" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="H130" s="18" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="J130" s="2" t="s">
         <v>76</v>
@@ -8772,13 +8771,13 @@
         <v>76</v>
       </c>
       <c r="N130" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O130" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P130" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q130" s="2"/>
       <c r="R130" s="20"/>
@@ -8811,7 +8810,7 @@
         <v>213</v>
       </c>
       <c r="K131" s="24" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="L131" s="2"/>
       <c r="M131" s="2"/>
@@ -18034,11 +18033,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T131" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="19">
-      <filters>
-        <filter val="KO"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:T131">
       <sortCondition ref="A9:A131"/>
     </sortState>

</xml_diff>

<commit_message>
Aggiunti i Data.json  e  report-CheckList
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DTSCONSULTI/DTSCONSULTINGSRL/DTSHIS/1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111DTSCONSULTI/DTSCONSULTINGSRL/DTSHIS/1.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc utente\Desktop\GATEWAY\S1#111DTSCONSULTI\DTSCONSULTINGSRL\DTSHIS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90CFA66-1973-4ECA-B36E-0152573770C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB511EEC-2484-45B1-B4F2-85A33A237D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -832,9 +832,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.2e536b3745^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>ef8bbca283018805</t>
-  </si>
-  <si>
     <t>2023-05-11T17:36:52Z</t>
   </si>
   <si>
@@ -1786,12 +1783,6 @@
     <t>2023-06-09T14:59:42Z</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.73edf2fd9b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-09T15:26:25Z</t>
-  </si>
-  <si>
     <t>8c28240b6d3c06c9</t>
   </si>
   <si>
@@ -1801,22 +1792,31 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.1803f2626d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>a645b0a2a1c3b61f</t>
-  </si>
-  <si>
-    <t>2023-06-09T18:21:40Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.d8eb0b0c9f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>9dee1b038c62ae5d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.6e01010233^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-06-09T18:22:40Z</t>
+    <t>cb196407773e51f2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.654ff17b70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-15T11:35:25Z</t>
+  </si>
+  <si>
+    <t>a6a7f97d42a393eb</t>
+  </si>
+  <si>
+    <t>2023-06-19T17:26:40Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.645f4530e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>080c93df9d635107</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.30518b672e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-19T17:29:40Z</t>
   </si>
 </sst>
 </file>
@@ -2495,10 +2495,10 @@
   <dimension ref="A1:T726"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G138" sqref="G138"/>
+      <selection pane="bottomRight" activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="91.7109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2909,16 +2909,16 @@
         <v>37</v>
       </c>
       <c r="F13" s="17">
-        <v>45086</v>
+        <v>45092</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>227</v>
+        <v>518</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>76</v>
@@ -2956,13 +2956,13 @@
         <v>45057</v>
       </c>
       <c r="G14" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="H14" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="I14" s="19" t="s">
         <v>229</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>230</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>76</v>
@@ -3000,13 +3000,13 @@
         <v>45063</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>76</v>
@@ -3044,13 +3044,13 @@
         <v>45063</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>76</v>
@@ -3088,13 +3088,13 @@
         <v>45063</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>76</v>
@@ -3132,13 +3132,13 @@
         <v>45063</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>76</v>
@@ -3176,13 +3176,13 @@
         <v>45062</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H19" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="I19" s="23" t="s">
         <v>261</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>262</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>76</v>
@@ -3220,13 +3220,13 @@
         <v>45062</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H20" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="I20" s="23" t="s">
         <v>263</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>264</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>76</v>
@@ -3268,7 +3268,7 @@
         <v>213</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -3306,7 +3306,7 @@
         <v>213</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -3340,13 +3340,13 @@
         <v>45086</v>
       </c>
       <c r="G23" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="I23" s="18" t="s">
         <v>511</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>510</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>512</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>76</v>
@@ -3384,13 +3384,13 @@
         <v>45063</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H24" s="18" t="s">
+        <v>419</v>
+      </c>
+      <c r="I24" s="18" t="s">
         <v>420</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>421</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>76</v>
@@ -3428,13 +3428,13 @@
         <v>45086</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>76</v>
@@ -3472,13 +3472,13 @@
         <v>45063</v>
       </c>
       <c r="G26" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="H26" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="H26" s="18" t="s">
-        <v>419</v>
-      </c>
       <c r="I26" s="18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>76</v>
@@ -3510,7 +3510,7 @@
         <v>64</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
@@ -3520,14 +3520,14 @@
         <v>213</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="20"/>
@@ -3550,7 +3550,7 @@
         <v>65</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
@@ -3560,14 +3560,14 @@
         <v>213</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="20"/>
@@ -3590,7 +3590,7 @@
         <v>66</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
@@ -3600,14 +3600,14 @@
         <v>213</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="20"/>
@@ -3630,7 +3630,7 @@
         <v>67</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
@@ -3640,14 +3640,14 @@
         <v>213</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="20"/>
@@ -3670,7 +3670,7 @@
         <v>68</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="18"/>
@@ -3680,14 +3680,14 @@
         <v>213</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="20"/>
@@ -3710,19 +3710,19 @@
         <v>69</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F32" s="17">
         <v>45062</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>76</v>
@@ -3735,13 +3735,13 @@
         <v>76</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="20"/>
@@ -3764,19 +3764,19 @@
         <v>70</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F33" s="17">
         <v>45063</v>
       </c>
       <c r="G33" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="H33" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="H33" s="18" t="s">
-        <v>366</v>
-      </c>
       <c r="I33" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>76</v>
@@ -3789,13 +3789,13 @@
         <v>76</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="20"/>
@@ -3818,22 +3818,22 @@
         <v>71</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F34" s="17">
         <v>45062</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
@@ -3843,13 +3843,13 @@
         <v>76</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O34" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="20"/>
@@ -3872,19 +3872,19 @@
         <v>72</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F35" s="17">
         <v>45062</v>
       </c>
       <c r="G35" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="H35" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="H35" s="18" t="s">
-        <v>364</v>
-      </c>
       <c r="I35" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>76</v>
@@ -3897,13 +3897,13 @@
         <v>76</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O35" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="20"/>
@@ -3926,19 +3926,19 @@
         <v>73</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F36" s="17">
         <v>45063</v>
       </c>
       <c r="G36" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="H36" s="18" t="s">
         <v>415</v>
       </c>
-      <c r="H36" s="18" t="s">
-        <v>416</v>
-      </c>
       <c r="I36" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>76</v>
@@ -3951,13 +3951,13 @@
         <v>76</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O36" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="20"/>
@@ -3997,11 +3997,11 @@
         <v>76</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="20"/>
@@ -4037,7 +4037,7 @@
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="20" t="s">
@@ -4075,7 +4075,7 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q39" s="2"/>
       <c r="R39" s="20" t="s">
@@ -4113,7 +4113,7 @@
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q40" s="2"/>
       <c r="R40" s="20" t="s">
@@ -4151,7 +4151,7 @@
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="20" t="s">
@@ -4182,13 +4182,13 @@
         <v>45062</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H42" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="I42" s="19" t="s">
         <v>237</v>
-      </c>
-      <c r="I42" s="19" t="s">
-        <v>238</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>76</v>
@@ -4201,13 +4201,13 @@
         <v>76</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="20"/>
@@ -4236,13 +4236,13 @@
         <v>45062</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H43" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="I43" s="19" t="s">
         <v>240</v>
-      </c>
-      <c r="I43" s="19" t="s">
-        <v>241</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>76</v>
@@ -4255,13 +4255,13 @@
         <v>76</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O43" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="20"/>
@@ -4290,13 +4290,13 @@
         <v>45062</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H44" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="I44" s="19" t="s">
         <v>242</v>
-      </c>
-      <c r="I44" s="19" t="s">
-        <v>243</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>76</v>
@@ -4309,13 +4309,13 @@
         <v>76</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O44" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q44" s="2"/>
       <c r="R44" s="20"/>
@@ -4344,13 +4344,13 @@
         <v>45062</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H45" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="I45" s="19" t="s">
         <v>246</v>
-      </c>
-      <c r="I45" s="19" t="s">
-        <v>247</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>76</v>
@@ -4363,13 +4363,13 @@
         <v>76</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O45" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="20"/>
@@ -4398,13 +4398,13 @@
         <v>45072</v>
       </c>
       <c r="G46" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>498</v>
+      </c>
+      <c r="I46" s="19" t="s">
         <v>500</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>499</v>
-      </c>
-      <c r="I46" s="19" t="s">
-        <v>501</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>76</v>
@@ -4417,13 +4417,13 @@
         <v>76</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q46" s="2"/>
       <c r="R46" s="20"/>
@@ -4452,13 +4452,13 @@
         <v>45062</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H47" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="I47" s="19" t="s">
         <v>248</v>
-      </c>
-      <c r="I47" s="19" t="s">
-        <v>249</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>76</v>
@@ -4471,13 +4471,13 @@
         <v>76</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O47" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="20"/>
@@ -4506,13 +4506,13 @@
         <v>45062</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H48" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="I48" s="19" t="s">
         <v>252</v>
-      </c>
-      <c r="I48" s="19" t="s">
-        <v>253</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>76</v>
@@ -4525,13 +4525,13 @@
         <v>76</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q48" s="2"/>
       <c r="R48" s="20"/>
@@ -4560,13 +4560,13 @@
         <v>45072</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>76</v>
@@ -4579,13 +4579,13 @@
         <v>76</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q49" s="2"/>
       <c r="R49" s="20"/>
@@ -4614,13 +4614,13 @@
         <v>45062</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H50" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="I50" s="19" t="s">
         <v>254</v>
-      </c>
-      <c r="I50" s="19" t="s">
-        <v>255</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>76</v>
@@ -4633,13 +4633,13 @@
         <v>76</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q50" s="2"/>
       <c r="R50" s="20"/>
@@ -4668,13 +4668,13 @@
         <v>45062</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H51" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="I51" s="19" t="s">
         <v>256</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>257</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>76</v>
@@ -4687,13 +4687,13 @@
         <v>76</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O51" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q51" s="2"/>
       <c r="R51" s="20"/>
@@ -4722,13 +4722,13 @@
         <v>45072</v>
       </c>
       <c r="G52" s="18" t="s">
+        <v>504</v>
+      </c>
+      <c r="H52" s="18" t="s">
         <v>505</v>
       </c>
-      <c r="H52" s="18" t="s">
+      <c r="I52" s="19" t="s">
         <v>506</v>
-      </c>
-      <c r="I52" s="19" t="s">
-        <v>507</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>76</v>
@@ -4741,13 +4741,13 @@
         <v>76</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O52" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q52" s="2"/>
       <c r="R52" s="20"/>
@@ -4776,13 +4776,13 @@
         <v>45063</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H53" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="I53" s="23" t="s">
         <v>402</v>
-      </c>
-      <c r="I53" s="23" t="s">
-        <v>403</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>76</v>
@@ -4795,13 +4795,13 @@
         <v>76</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O53" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q53" s="2"/>
       <c r="R53" s="20"/>
@@ -4830,13 +4830,13 @@
         <v>45063</v>
       </c>
       <c r="G54" s="18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>76</v>
@@ -4849,13 +4849,13 @@
         <v>76</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O54" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q54" s="2"/>
       <c r="R54" s="20"/>
@@ -4884,13 +4884,13 @@
         <v>45063</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>76</v>
@@ -4903,13 +4903,13 @@
         <v>76</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q55" s="2"/>
       <c r="R55" s="20"/>
@@ -4938,13 +4938,13 @@
         <v>45063</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>76</v>
@@ -4957,13 +4957,13 @@
         <v>76</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O56" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" s="20"/>
@@ -4992,13 +4992,13 @@
         <v>45063</v>
       </c>
       <c r="G57" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>76</v>
@@ -5011,13 +5011,13 @@
         <v>76</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q57" s="2"/>
       <c r="R57" s="20"/>
@@ -5046,13 +5046,13 @@
         <v>45063</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I58" s="23" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>76</v>
@@ -5065,13 +5065,13 @@
         <v>76</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O58" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" s="20"/>
@@ -5100,13 +5100,13 @@
         <v>45063</v>
       </c>
       <c r="G59" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>76</v>
@@ -5119,13 +5119,13 @@
         <v>76</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="20"/>
@@ -5154,13 +5154,13 @@
         <v>45063</v>
       </c>
       <c r="G60" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>76</v>
@@ -5173,13 +5173,13 @@
         <v>76</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O60" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="20"/>
@@ -5208,13 +5208,13 @@
         <v>45063</v>
       </c>
       <c r="G61" s="18" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>76</v>
@@ -5227,13 +5227,13 @@
         <v>76</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P61" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="20"/>
@@ -5262,13 +5262,13 @@
         <v>45063</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>76</v>
@@ -5281,13 +5281,13 @@
         <v>76</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O62" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="20"/>
@@ -5316,13 +5316,13 @@
         <v>45063</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>76</v>
@@ -5335,13 +5335,13 @@
         <v>76</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O63" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q63" s="2"/>
       <c r="R63" s="20"/>
@@ -5370,13 +5370,13 @@
         <v>45063</v>
       </c>
       <c r="G64" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="H64" s="18" t="s">
         <v>390</v>
       </c>
-      <c r="H64" s="18" t="s">
-        <v>391</v>
-      </c>
       <c r="I64" s="23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>76</v>
@@ -5389,13 +5389,13 @@
         <v>76</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O64" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q64" s="2"/>
       <c r="R64" s="20"/>
@@ -5424,13 +5424,13 @@
         <v>45062</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H65" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="I65" s="23" t="s">
         <v>279</v>
-      </c>
-      <c r="I65" s="23" t="s">
-        <v>280</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>76</v>
@@ -5443,13 +5443,13 @@
         <v>76</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O65" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P65" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q65" s="2"/>
       <c r="R65" s="20"/>
@@ -5478,13 +5478,13 @@
         <v>45062</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>76</v>
@@ -5497,13 +5497,13 @@
         <v>76</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O66" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q66" s="2"/>
       <c r="R66" s="20"/>
@@ -5532,13 +5532,13 @@
         <v>45062</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>76</v>
@@ -5551,13 +5551,13 @@
         <v>76</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O67" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q67" s="2"/>
       <c r="R67" s="20"/>
@@ -5586,13 +5586,13 @@
         <v>45062</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I68" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>76</v>
@@ -5605,13 +5605,13 @@
         <v>76</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O68" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P68" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="20"/>
@@ -5640,13 +5640,13 @@
         <v>45062</v>
       </c>
       <c r="G69" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="H69" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="H69" s="18" t="s">
-        <v>275</v>
-      </c>
       <c r="I69" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>76</v>
@@ -5659,13 +5659,13 @@
         <v>76</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O69" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P69" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="20"/>
@@ -5694,13 +5694,13 @@
         <v>45062</v>
       </c>
       <c r="G70" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H70" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="I70" s="23" t="s">
         <v>289</v>
-      </c>
-      <c r="I70" s="23" t="s">
-        <v>290</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>76</v>
@@ -5713,13 +5713,13 @@
         <v>76</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O70" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="20"/>
@@ -5748,13 +5748,13 @@
         <v>45062</v>
       </c>
       <c r="G71" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="H71" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="H71" s="18" t="s">
-        <v>288</v>
-      </c>
       <c r="I71" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>76</v>
@@ -5767,13 +5767,13 @@
         <v>76</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O71" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q71" s="2"/>
       <c r="R71" s="20"/>
@@ -5802,13 +5802,13 @@
         <v>45062</v>
       </c>
       <c r="G72" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H72" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="I72" s="23" t="s">
         <v>301</v>
-      </c>
-      <c r="I72" s="23" t="s">
-        <v>302</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>76</v>
@@ -5821,13 +5821,13 @@
         <v>76</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O72" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P72" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q72" s="2"/>
       <c r="R72" s="20"/>
@@ -5856,13 +5856,13 @@
         <v>45062</v>
       </c>
       <c r="G73" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I73" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>76</v>
@@ -5875,13 +5875,13 @@
         <v>76</v>
       </c>
       <c r="N73" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O73" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P73" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q73" s="2"/>
       <c r="R73" s="20"/>
@@ -5910,13 +5910,13 @@
         <v>45062</v>
       </c>
       <c r="G74" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H74" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I74" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>76</v>
@@ -5929,13 +5929,13 @@
         <v>76</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O74" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P74" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q74" s="2"/>
       <c r="R74" s="20"/>
@@ -5964,13 +5964,13 @@
         <v>45062</v>
       </c>
       <c r="G75" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I75" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>76</v>
@@ -5983,13 +5983,13 @@
         <v>76</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O75" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q75" s="2"/>
       <c r="R75" s="20"/>
@@ -6018,13 +6018,13 @@
         <v>45062</v>
       </c>
       <c r="G76" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="H76" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="H76" s="18" t="s">
-        <v>297</v>
-      </c>
       <c r="I76" s="23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>76</v>
@@ -6037,13 +6037,13 @@
         <v>76</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O76" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q76" s="2"/>
       <c r="R76" s="20"/>
@@ -6076,12 +6076,12 @@
         <v>213</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
@@ -6116,12 +6116,12 @@
         <v>213</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
@@ -6156,12 +6156,12 @@
         <v>213</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
@@ -6196,12 +6196,12 @@
         <v>213</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
       <c r="N80" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
@@ -6236,12 +6236,12 @@
         <v>213</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
@@ -6272,13 +6272,13 @@
         <v>45062</v>
       </c>
       <c r="G82" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="H82" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="H82" s="18" t="s">
+      <c r="I82" s="23" t="s">
         <v>310</v>
-      </c>
-      <c r="I82" s="23" t="s">
-        <v>311</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>76</v>
@@ -6291,13 +6291,13 @@
         <v>76</v>
       </c>
       <c r="N82" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O82" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P82" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q82" s="2"/>
       <c r="R82" s="20"/>
@@ -6326,13 +6326,13 @@
         <v>45062</v>
       </c>
       <c r="G83" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="H83" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="H83" s="18" t="s">
-        <v>308</v>
-      </c>
       <c r="I83" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>76</v>
@@ -6345,13 +6345,13 @@
         <v>76</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O83" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P83" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q83" s="2"/>
       <c r="R83" s="20"/>
@@ -6380,13 +6380,13 @@
         <v>45063</v>
       </c>
       <c r="G84" s="18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H84" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="I84" s="23" t="s">
         <v>434</v>
-      </c>
-      <c r="I84" s="23" t="s">
-        <v>435</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>76</v>
@@ -6399,13 +6399,13 @@
         <v>76</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O84" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P84" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q84" s="2"/>
       <c r="R84" s="20"/>
@@ -6434,13 +6434,13 @@
         <v>45063</v>
       </c>
       <c r="G85" s="18" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H85" s="18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>76</v>
@@ -6453,13 +6453,13 @@
         <v>76</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O85" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P85" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q85" s="2"/>
       <c r="R85" s="20"/>
@@ -6488,13 +6488,13 @@
         <v>45063</v>
       </c>
       <c r="G86" s="18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H86" s="18" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>76</v>
@@ -6507,13 +6507,13 @@
         <v>76</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O86" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P86" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q86" s="2"/>
       <c r="R86" s="20"/>
@@ -6542,13 +6542,13 @@
         <v>45063</v>
       </c>
       <c r="G87" s="18" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H87" s="18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>76</v>
@@ -6561,13 +6561,13 @@
         <v>76</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O87" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P87" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q87" s="2"/>
       <c r="R87" s="20"/>
@@ -6596,13 +6596,13 @@
         <v>45063</v>
       </c>
       <c r="G88" s="18" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H88" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I88" s="23" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>76</v>
@@ -6615,13 +6615,13 @@
         <v>76</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O88" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P88" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q88" s="2"/>
       <c r="R88" s="20"/>
@@ -6650,13 +6650,13 @@
         <v>45063</v>
       </c>
       <c r="G89" s="18" t="s">
+        <v>427</v>
+      </c>
+      <c r="H89" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="H89" s="18" t="s">
-        <v>429</v>
-      </c>
       <c r="I89" s="23" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>76</v>
@@ -6669,13 +6669,13 @@
         <v>76</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O89" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P89" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q89" s="2"/>
       <c r="R89" s="20"/>
@@ -6704,13 +6704,13 @@
         <v>45063</v>
       </c>
       <c r="G90" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="H90" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="I90" s="23" t="s">
         <v>442</v>
-      </c>
-      <c r="H90" s="18" t="s">
-        <v>441</v>
-      </c>
-      <c r="I90" s="23" t="s">
-        <v>443</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>76</v>
@@ -6723,13 +6723,13 @@
         <v>76</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q90" s="2"/>
       <c r="R90" s="20"/>
@@ -6758,13 +6758,13 @@
         <v>45064</v>
       </c>
       <c r="G91" s="18" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H91" s="18" t="s">
+        <v>450</v>
+      </c>
+      <c r="I91" s="23" t="s">
         <v>451</v>
-      </c>
-      <c r="I91" s="23" t="s">
-        <v>452</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>76</v>
@@ -6777,13 +6777,13 @@
         <v>76</v>
       </c>
       <c r="N91" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O91" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P91" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q91" s="2"/>
       <c r="R91" s="20"/>
@@ -6812,13 +6812,13 @@
         <v>45064</v>
       </c>
       <c r="G92" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H92" s="18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I92" s="23" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>76</v>
@@ -6831,13 +6831,13 @@
         <v>76</v>
       </c>
       <c r="N92" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O92" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q92" s="2"/>
       <c r="R92" s="20"/>
@@ -6866,13 +6866,13 @@
         <v>45064</v>
       </c>
       <c r="G93" s="18" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H93" s="18" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I93" s="23" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>76</v>
@@ -6885,13 +6885,13 @@
         <v>76</v>
       </c>
       <c r="N93" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O93" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q93" s="2"/>
       <c r="R93" s="20"/>
@@ -6920,13 +6920,13 @@
         <v>45064</v>
       </c>
       <c r="G94" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="H94" s="18" t="s">
         <v>447</v>
       </c>
-      <c r="H94" s="18" t="s">
-        <v>448</v>
-      </c>
       <c r="I94" s="23" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>76</v>
@@ -6939,13 +6939,13 @@
         <v>76</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O94" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P94" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q94" s="2"/>
       <c r="R94" s="20"/>
@@ -6974,13 +6974,13 @@
         <v>45064</v>
       </c>
       <c r="G95" s="18" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H95" s="18" t="s">
+        <v>458</v>
+      </c>
+      <c r="I95" s="23" t="s">
         <v>459</v>
-      </c>
-      <c r="I95" s="23" t="s">
-        <v>460</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>76</v>
@@ -6993,13 +6993,13 @@
         <v>76</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O95" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P95" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q95" s="2"/>
       <c r="R95" s="20"/>
@@ -7028,13 +7028,13 @@
         <v>45064</v>
       </c>
       <c r="G96" s="18" t="s">
+        <v>456</v>
+      </c>
+      <c r="H96" s="18" t="s">
         <v>457</v>
       </c>
-      <c r="H96" s="18" t="s">
-        <v>458</v>
-      </c>
       <c r="I96" s="23" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>76</v>
@@ -7047,13 +7047,13 @@
         <v>76</v>
       </c>
       <c r="N96" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O96" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P96" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q96" s="2"/>
       <c r="R96" s="20"/>
@@ -7082,13 +7082,13 @@
         <v>45064</v>
       </c>
       <c r="G97" s="18" t="s">
+        <v>461</v>
+      </c>
+      <c r="H97" s="18" t="s">
         <v>462</v>
       </c>
-      <c r="H97" s="18" t="s">
+      <c r="I97" s="23" t="s">
         <v>463</v>
-      </c>
-      <c r="I97" s="23" t="s">
-        <v>464</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>76</v>
@@ -7101,13 +7101,13 @@
         <v>76</v>
       </c>
       <c r="N97" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O97" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P97" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q97" s="2"/>
       <c r="R97" s="20"/>
@@ -7136,13 +7136,13 @@
         <v>45064</v>
       </c>
       <c r="G98" s="18" t="s">
+        <v>464</v>
+      </c>
+      <c r="H98" s="18" t="s">
         <v>465</v>
       </c>
-      <c r="H98" s="18" t="s">
+      <c r="I98" s="23" t="s">
         <v>466</v>
-      </c>
-      <c r="I98" s="23" t="s">
-        <v>467</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>76</v>
@@ -7155,13 +7155,13 @@
         <v>76</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O98" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P98" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q98" s="2"/>
       <c r="R98" s="20"/>
@@ -7190,13 +7190,13 @@
         <v>45064</v>
       </c>
       <c r="G99" s="18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H99" s="18" t="s">
+        <v>470</v>
+      </c>
+      <c r="I99" s="23" t="s">
         <v>471</v>
-      </c>
-      <c r="I99" s="23" t="s">
-        <v>472</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>76</v>
@@ -7209,13 +7209,13 @@
         <v>76</v>
       </c>
       <c r="N99" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O99" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P99" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q99" s="2"/>
       <c r="R99" s="20"/>
@@ -7244,13 +7244,13 @@
         <v>45064</v>
       </c>
       <c r="G100" s="18" t="s">
+        <v>468</v>
+      </c>
+      <c r="H100" s="18" t="s">
         <v>469</v>
       </c>
-      <c r="H100" s="18" t="s">
-        <v>470</v>
-      </c>
       <c r="I100" s="23" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>76</v>
@@ -7263,13 +7263,13 @@
         <v>76</v>
       </c>
       <c r="N100" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O100" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P100" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q100" s="2"/>
       <c r="R100" s="20"/>
@@ -7298,13 +7298,13 @@
         <v>45064</v>
       </c>
       <c r="G101" s="18" t="s">
+        <v>473</v>
+      </c>
+      <c r="H101" s="18" t="s">
         <v>474</v>
       </c>
-      <c r="H101" s="18" t="s">
+      <c r="I101" s="23" t="s">
         <v>475</v>
-      </c>
-      <c r="I101" s="23" t="s">
-        <v>476</v>
       </c>
       <c r="J101" s="2" t="s">
         <v>76</v>
@@ -7317,13 +7317,13 @@
         <v>76</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O101" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P101" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q101" s="2"/>
       <c r="R101" s="20"/>
@@ -7352,13 +7352,13 @@
         <v>45064</v>
       </c>
       <c r="G102" s="18" t="s">
+        <v>476</v>
+      </c>
+      <c r="H102" s="18" t="s">
         <v>477</v>
       </c>
-      <c r="H102" s="18" t="s">
+      <c r="I102" s="23" t="s">
         <v>478</v>
-      </c>
-      <c r="I102" s="23" t="s">
-        <v>479</v>
       </c>
       <c r="J102" s="2" t="s">
         <v>76</v>
@@ -7371,13 +7371,13 @@
         <v>76</v>
       </c>
       <c r="N102" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O102" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P102" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q102" s="2"/>
       <c r="R102" s="20"/>
@@ -7406,13 +7406,13 @@
         <v>45064</v>
       </c>
       <c r="G103" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="H103" s="18" t="s">
         <v>480</v>
       </c>
-      <c r="H103" s="18" t="s">
+      <c r="I103" s="23" t="s">
         <v>481</v>
-      </c>
-      <c r="I103" s="23" t="s">
-        <v>482</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>76</v>
@@ -7425,13 +7425,13 @@
         <v>76</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O103" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P103" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q103" s="2"/>
       <c r="R103" s="20"/>
@@ -7460,13 +7460,13 @@
         <v>45065</v>
       </c>
       <c r="G104" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="H104" s="18" t="s">
         <v>486</v>
       </c>
-      <c r="H104" s="18" t="s">
+      <c r="I104" s="23" t="s">
         <v>487</v>
-      </c>
-      <c r="I104" s="23" t="s">
-        <v>488</v>
       </c>
       <c r="J104" s="2" t="s">
         <v>76</v>
@@ -7479,13 +7479,13 @@
         <v>76</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O104" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P104" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q104" s="2"/>
       <c r="R104" s="20"/>
@@ -7514,13 +7514,13 @@
         <v>45065</v>
       </c>
       <c r="G105" s="18" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H105" s="18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I105" s="23" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J105" s="2" t="s">
         <v>76</v>
@@ -7533,13 +7533,13 @@
         <v>76</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O105" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P105" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q105" s="2"/>
       <c r="R105" s="20"/>
@@ -7568,13 +7568,13 @@
         <v>45065</v>
       </c>
       <c r="G106" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="H106" s="18" t="s">
         <v>492</v>
       </c>
-      <c r="H106" s="18" t="s">
+      <c r="I106" s="23" t="s">
         <v>493</v>
-      </c>
-      <c r="I106" s="23" t="s">
-        <v>494</v>
       </c>
       <c r="J106" s="2" t="s">
         <v>76</v>
@@ -7587,13 +7587,13 @@
         <v>76</v>
       </c>
       <c r="N106" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O106" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P106" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q106" s="2"/>
       <c r="R106" s="20"/>
@@ -7622,13 +7622,13 @@
         <v>45065</v>
       </c>
       <c r="G107" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="H107" s="18" t="s">
         <v>483</v>
       </c>
-      <c r="H107" s="18" t="s">
+      <c r="I107" s="23" t="s">
         <v>484</v>
-      </c>
-      <c r="I107" s="23" t="s">
-        <v>485</v>
       </c>
       <c r="J107" s="2" t="s">
         <v>76</v>
@@ -7641,13 +7641,13 @@
         <v>76</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O107" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P107" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q107" s="2"/>
       <c r="R107" s="20"/>
@@ -7676,13 +7676,13 @@
         <v>45065</v>
       </c>
       <c r="G108" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="H108" s="18" t="s">
         <v>495</v>
       </c>
-      <c r="H108" s="18" t="s">
+      <c r="I108" s="23" t="s">
         <v>496</v>
-      </c>
-      <c r="I108" s="23" t="s">
-        <v>497</v>
       </c>
       <c r="J108" s="2" t="s">
         <v>76</v>
@@ -7695,13 +7695,13 @@
         <v>76</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O108" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P108" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q108" s="2"/>
       <c r="R108" s="20"/>
@@ -7728,13 +7728,13 @@
         <v>45062</v>
       </c>
       <c r="G109" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="H109" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="H109" s="18" t="s">
+      <c r="I109" s="19" t="s">
         <v>314</v>
-      </c>
-      <c r="I109" s="19" t="s">
-        <v>315</v>
       </c>
       <c r="J109" s="2" t="s">
         <v>76</v>
@@ -7770,13 +7770,13 @@
         <v>45086</v>
       </c>
       <c r="G110" s="18" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="H110" s="18" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="I110" s="19" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="J110" s="2" t="s">
         <v>76</v>
@@ -7809,7 +7809,7 @@
       </c>
       <c r="E111" s="16"/>
       <c r="F111" s="17">
-        <v>45086</v>
+        <v>45096</v>
       </c>
       <c r="G111" s="18" t="s">
         <v>522</v>
@@ -7851,7 +7851,7 @@
       </c>
       <c r="E112" s="16"/>
       <c r="F112" s="17">
-        <v>45086</v>
+        <v>45096</v>
       </c>
       <c r="G112" s="18" t="s">
         <v>526</v>
@@ -7898,13 +7898,13 @@
         <v>45062</v>
       </c>
       <c r="G113" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H113" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="I113" s="19" t="s">
         <v>320</v>
-      </c>
-      <c r="I113" s="19" t="s">
-        <v>321</v>
       </c>
       <c r="J113" s="2" t="s">
         <v>76</v>
@@ -7917,13 +7917,13 @@
         <v>76</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O113" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P113" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q113" s="2"/>
       <c r="R113" s="20"/>
@@ -7952,13 +7952,13 @@
         <v>45062</v>
       </c>
       <c r="G114" s="18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H114" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="I114" s="19" t="s">
         <v>322</v>
-      </c>
-      <c r="I114" s="19" t="s">
-        <v>323</v>
       </c>
       <c r="J114" s="2" t="s">
         <v>76</v>
@@ -7971,13 +7971,13 @@
         <v>76</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O114" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P114" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q114" s="2"/>
       <c r="R114" s="20"/>
@@ -8006,13 +8006,13 @@
         <v>45062</v>
       </c>
       <c r="G115" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="H115" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="H115" s="18" t="s">
+      <c r="I115" s="19" t="s">
         <v>325</v>
-      </c>
-      <c r="I115" s="19" t="s">
-        <v>326</v>
       </c>
       <c r="J115" s="2" t="s">
         <v>76</v>
@@ -8025,13 +8025,13 @@
         <v>76</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O115" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P115" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q115" s="2"/>
       <c r="R115" s="20"/>
@@ -8060,13 +8060,13 @@
         <v>45062</v>
       </c>
       <c r="G116" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="H116" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="H116" s="18" t="s">
+      <c r="I116" s="19" t="s">
         <v>328</v>
-      </c>
-      <c r="I116" s="19" t="s">
-        <v>329</v>
       </c>
       <c r="J116" s="2" t="s">
         <v>76</v>
@@ -8079,13 +8079,13 @@
         <v>76</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O116" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P116" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q116" s="2"/>
       <c r="R116" s="20"/>
@@ -8114,13 +8114,13 @@
         <v>45062</v>
       </c>
       <c r="G117" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="H117" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="H117" s="18" t="s">
+      <c r="I117" s="19" t="s">
         <v>331</v>
-      </c>
-      <c r="I117" s="19" t="s">
-        <v>332</v>
       </c>
       <c r="J117" s="2" t="s">
         <v>76</v>
@@ -8133,13 +8133,13 @@
         <v>76</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O117" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P117" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q117" s="2"/>
       <c r="R117" s="20"/>
@@ -8168,13 +8168,13 @@
         <v>45062</v>
       </c>
       <c r="G118" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="H118" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="H118" s="18" t="s">
+      <c r="I118" s="19" t="s">
         <v>334</v>
-      </c>
-      <c r="I118" s="19" t="s">
-        <v>335</v>
       </c>
       <c r="J118" s="2" t="s">
         <v>76</v>
@@ -8187,13 +8187,13 @@
         <v>76</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O118" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P118" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q118" s="2"/>
       <c r="R118" s="20"/>
@@ -8222,13 +8222,13 @@
         <v>45062</v>
       </c>
       <c r="G119" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H119" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="I119" s="19" t="s">
         <v>341</v>
-      </c>
-      <c r="I119" s="19" t="s">
-        <v>342</v>
       </c>
       <c r="J119" s="2" t="s">
         <v>76</v>
@@ -8241,13 +8241,13 @@
         <v>76</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O119" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P119" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q119" s="2"/>
       <c r="R119" s="20"/>
@@ -8276,13 +8276,13 @@
         <v>45062</v>
       </c>
       <c r="G120" s="18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H120" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I120" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J120" s="2" t="s">
         <v>76</v>
@@ -8295,13 +8295,13 @@
         <v>76</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O120" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P120" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q120" s="2"/>
       <c r="R120" s="20"/>
@@ -8330,13 +8330,13 @@
         <v>45062</v>
       </c>
       <c r="G121" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="H121" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="H121" s="18" t="s">
-        <v>339</v>
-      </c>
       <c r="I121" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J121" s="2" t="s">
         <v>76</v>
@@ -8349,13 +8349,13 @@
         <v>76</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O121" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P121" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q121" s="2"/>
       <c r="R121" s="20"/>
@@ -8384,13 +8384,13 @@
         <v>45063</v>
       </c>
       <c r="G122" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H122" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I122" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J122" s="2" t="s">
         <v>76</v>
@@ -8403,13 +8403,13 @@
         <v>76</v>
       </c>
       <c r="N122" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O122" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P122" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q122" s="2"/>
       <c r="R122" s="20"/>
@@ -8438,13 +8438,13 @@
         <v>45063</v>
       </c>
       <c r="G123" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="H123" s="18" t="s">
         <v>346</v>
       </c>
-      <c r="H123" s="18" t="s">
+      <c r="I123" s="19" t="s">
         <v>347</v>
-      </c>
-      <c r="I123" s="19" t="s">
-        <v>348</v>
       </c>
       <c r="J123" s="2" t="s">
         <v>76</v>
@@ -8457,13 +8457,13 @@
         <v>76</v>
       </c>
       <c r="N123" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O123" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P123" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q123" s="2"/>
       <c r="R123" s="20"/>
@@ -8492,13 +8492,13 @@
         <v>45063</v>
       </c>
       <c r="G124" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="H124" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="H124" s="18" t="s">
+      <c r="I124" s="19" t="s">
         <v>352</v>
-      </c>
-      <c r="I124" s="19" t="s">
-        <v>353</v>
       </c>
       <c r="J124" s="2" t="s">
         <v>76</v>
@@ -8511,13 +8511,13 @@
         <v>76</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O124" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P124" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q124" s="2"/>
       <c r="R124" s="20"/>
@@ -8546,13 +8546,13 @@
         <v>45063</v>
       </c>
       <c r="G125" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H125" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="I125" s="19" t="s">
         <v>354</v>
-      </c>
-      <c r="I125" s="19" t="s">
-        <v>355</v>
       </c>
       <c r="J125" s="2" t="s">
         <v>76</v>
@@ -8565,13 +8565,13 @@
         <v>76</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O125" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P125" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q125" s="2"/>
       <c r="R125" s="20"/>
@@ -8604,7 +8604,7 @@
         <v>213</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L126" s="2"/>
       <c r="M126" s="2"/>
@@ -8642,7 +8642,7 @@
         <v>213</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L127" s="2"/>
       <c r="M127" s="2"/>
@@ -8680,7 +8680,7 @@
         <v>213</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L128" s="2"/>
       <c r="M128" s="2"/>
@@ -8718,7 +8718,7 @@
         <v>213</v>
       </c>
       <c r="K129" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L129" s="2"/>
       <c r="M129" s="2"/>
@@ -8752,13 +8752,13 @@
         <v>45063</v>
       </c>
       <c r="G130" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="H130" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="H130" s="18" t="s">
+      <c r="I130" s="19" t="s">
         <v>360</v>
-      </c>
-      <c r="I130" s="19" t="s">
-        <v>361</v>
       </c>
       <c r="J130" s="2" t="s">
         <v>76</v>
@@ -8771,13 +8771,13 @@
         <v>76</v>
       </c>
       <c r="N130" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O130" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P130" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q130" s="2"/>
       <c r="R130" s="20"/>
@@ -8810,7 +8810,7 @@
         <v>213</v>
       </c>
       <c r="K131" s="24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L131" s="2"/>
       <c r="M131" s="2"/>

</xml_diff>